<commit_message>
updated bar chart logic in the HPI, LPI, and LPNI reports
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2656 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: fab994b4cc2210699c8bc9f73d2cd2ca31f92f6f
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="95">
   <si>
     <t>Garrison / Theater</t>
   </si>
@@ -427,6 +427,9 @@
   </si>
   <si>
     <t>Example Site Name</t>
+  </si>
+  <si>
+    <t>Proposed Temporary Interfaces with DHMSM - Legacy Consumer</t>
   </si>
 </sst>
 </file>
@@ -1021,6 +1024,45 @@
     <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1048,15 +1090,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1066,28 +1099,10 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1185,18 +1200,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1472,11 +1475,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="436811648"/>
-        <c:axId val="436812040"/>
+        <c:axId val="466315792"/>
+        <c:axId val="466315400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="436811648"/>
+        <c:axId val="466315792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1486,7 +1489,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="436812040"/>
+        <c:crossAx val="466315400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1494,7 +1497,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="436812040"/>
+        <c:axId val="466315400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1505,7 +1508,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="436811648"/>
+        <c:crossAx val="466315792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1638,11 +1641,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="436814392"/>
-        <c:axId val="436814784"/>
+        <c:axId val="466315008"/>
+        <c:axId val="497266952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="436814392"/>
+        <c:axId val="466315008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1652,7 +1655,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="436814784"/>
+        <c:crossAx val="497266952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1660,7 +1663,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="436814784"/>
+        <c:axId val="497266952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1671,7 +1674,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="436814392"/>
+        <c:crossAx val="466315008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1904,6 +1907,45 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Summary Charts'!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Proposed Temporary Interfaces with DHMSM - Legacy Consumer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Summary Charts'!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Summary Charts'!$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1913,11 +1955,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="436815568"/>
-        <c:axId val="436815960"/>
+        <c:axId val="497267736"/>
+        <c:axId val="497268128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="436815568"/>
+        <c:axId val="497267736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1927,7 +1969,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="436815960"/>
+        <c:crossAx val="497268128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1935,7 +1977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="436815960"/>
+        <c:axId val="497268128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1946,7 +1988,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="436815568"/>
+        <c:crossAx val="497267736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -44656,10 +44698,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -44812,6 +44854,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="40">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
@@ -44827,7 +44877,7 @@
   <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54:E54"/>
+      <selection activeCell="O54" sqref="O54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44847,22 +44897,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="261.75" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="69" t="s">
+      <c r="C2" s="67"/>
+      <c r="D2" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="71"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="70"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -44920,22 +44970,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="69" t="s">
+      <c r="C7" s="67"/>
+      <c r="D7" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="70"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="71"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="70"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -44946,112 +44996,112 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="61"/>
-      <c r="M9" s="62"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="75"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75" t="s">
+      <c r="C10" s="71"/>
+      <c r="D10" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="82"/>
-      <c r="F10" s="75" t="s">
+      <c r="E10" s="72"/>
+      <c r="F10" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="75"/>
-      <c r="H10" s="76" t="s">
+      <c r="G10" s="71"/>
+      <c r="H10" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75" t="s">
+      <c r="I10" s="86"/>
+      <c r="J10" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75" t="s">
+      <c r="K10" s="71"/>
+      <c r="L10" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="75"/>
+      <c r="M10" s="71"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="79"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="79"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="65"/>
     </row>
     <row r="13" spans="1:13" ht="16.5">
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
-      <c r="L13" s="61"/>
-      <c r="M13" s="62"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="74"/>
+      <c r="L13" s="74"/>
+      <c r="M13" s="75"/>
     </row>
     <row r="14" spans="1:13" ht="51" customHeight="1">
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
-      <c r="M14" s="68"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="81"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="82" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="72" t="s">
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="84"/>
+      <c r="H15" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="74"/>
+      <c r="I15" s="83"/>
+      <c r="J15" s="83"/>
+      <c r="K15" s="83"/>
+      <c r="L15" s="83"/>
+      <c r="M15" s="84"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="42"/>
@@ -45278,36 +45328,36 @@
       <c r="M31" s="50"/>
     </row>
     <row r="33" spans="2:13" ht="16.5">
-      <c r="B33" s="60" t="s">
+      <c r="B33" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="61"/>
-      <c r="L33" s="61"/>
-      <c r="M33" s="62"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="74"/>
+      <c r="L33" s="74"/>
+      <c r="M33" s="75"/>
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B34" s="63" t="s">
+      <c r="B34" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="64"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="64"/>
-      <c r="J34" s="64"/>
-      <c r="K34" s="64"/>
-      <c r="L34" s="64"/>
-      <c r="M34" s="65"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
+      <c r="L34" s="77"/>
+      <c r="M34" s="78"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="42"/>
@@ -45535,65 +45585,71 @@
     </row>
     <row r="52" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A52" s="7"/>
-      <c r="B52" s="60" t="s">
+      <c r="B52" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="C52" s="61"/>
-      <c r="D52" s="61"/>
-      <c r="E52" s="61"/>
-      <c r="F52" s="61"/>
-      <c r="G52" s="61"/>
-      <c r="H52" s="61"/>
-      <c r="I52" s="61"/>
-      <c r="J52" s="61"/>
-      <c r="K52" s="61"/>
-      <c r="L52" s="61"/>
-      <c r="M52" s="62"/>
+      <c r="C52" s="74"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="74"/>
+      <c r="H52" s="74"/>
+      <c r="I52" s="74"/>
+      <c r="J52" s="74"/>
+      <c r="K52" s="74"/>
+      <c r="L52" s="74"/>
+      <c r="M52" s="75"/>
     </row>
     <row r="53" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A53" s="7"/>
-      <c r="B53" s="115" t="s">
+      <c r="B53" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="116"/>
-      <c r="D53" s="116"/>
-      <c r="E53" s="117"/>
-      <c r="F53" s="115" t="s">
+      <c r="C53" s="61"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="62"/>
+      <c r="F53" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="G53" s="116"/>
-      <c r="H53" s="116"/>
-      <c r="I53" s="117"/>
-      <c r="J53" s="115" t="s">
+      <c r="G53" s="61"/>
+      <c r="H53" s="61"/>
+      <c r="I53" s="62"/>
+      <c r="J53" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="K53" s="116"/>
-      <c r="L53" s="116"/>
-      <c r="M53" s="117"/>
+      <c r="K53" s="61"/>
+      <c r="L53" s="61"/>
+      <c r="M53" s="62"/>
     </row>
     <row r="54" spans="1:13" ht="42.75" customHeight="1">
       <c r="A54" s="5"/>
-      <c r="B54" s="78"/>
-      <c r="C54" s="118"/>
-      <c r="D54" s="118"/>
-      <c r="E54" s="79"/>
-      <c r="F54" s="78"/>
-      <c r="G54" s="118"/>
-      <c r="H54" s="118"/>
-      <c r="I54" s="79"/>
-      <c r="J54" s="78"/>
-      <c r="K54" s="118"/>
-      <c r="L54" s="118"/>
-      <c r="M54" s="79"/>
+      <c r="B54" s="63"/>
+      <c r="C54" s="64"/>
+      <c r="D54" s="64"/>
+      <c r="E54" s="65"/>
+      <c r="F54" s="63"/>
+      <c r="G54" s="64"/>
+      <c r="H54" s="64"/>
+      <c r="I54" s="65"/>
+      <c r="J54" s="63"/>
+      <c r="K54" s="64"/>
+      <c r="L54" s="64"/>
+      <c r="M54" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="B52:M52"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -45607,18 +45663,12 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B52:M52"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="F54:I54"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45657,26 +45707,26 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
@@ -45684,15 +45734,15 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="90" t="s">
+      <c r="A5" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="92"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="96"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
@@ -45700,17 +45750,17 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="88"/>
-      <c r="C7" s="84" t="s">
+      <c r="B7" s="92"/>
+      <c r="C7" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="86"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="90"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
@@ -45793,50 +45843,50 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="95"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="99"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="90" t="s">
+      <c r="A5" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="92"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="96"/>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="96" t="s">
+      <c r="B7" s="93"/>
+      <c r="C7" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
     </row>
     <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="35" t="s">
@@ -45904,18 +45954,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
     </row>
     <row r="3" spans="1:10" ht="18">
       <c r="A3" s="12"/>
@@ -45925,17 +45975,17 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="101" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="99"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="103"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2"/>
@@ -46083,34 +46133,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1"/>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
     </row>
     <row r="4" spans="1:10" ht="53.25" customHeight="1">
       <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="105" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="103"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="107"/>
     </row>
     <row r="6" spans="1:10" ht="39.75" customHeight="1">
       <c r="A6" s="35" t="s">
@@ -46155,10 +46205,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="100"/>
+      <c r="B2" s="104"/>
     </row>
     <row r="3" spans="1:2" ht="18">
       <c r="A3" s="12"/>
@@ -46219,11 +46269,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -46234,10 +46284,10 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="101" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="99"/>
+      <c r="C4" s="103"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -46303,74 +46353,74 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1"/>
     <row r="2" spans="1:13" ht="18" customHeight="1">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="100"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
     </row>
     <row r="4" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A4" s="112" t="s">
+      <c r="A4" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="113"/>
-      <c r="C4" s="114"/>
-      <c r="D4" s="104" t="s">
+      <c r="B4" s="117"/>
+      <c r="C4" s="118"/>
+      <c r="D4" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
-      <c r="M4" s="106"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="110"/>
     </row>
     <row r="6" spans="1:13" ht="96.75" customHeight="1">
-      <c r="A6" s="107" t="s">
+      <c r="A6" s="111" t="s">
         <v>83</v>
       </c>
       <c r="B6" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
       <c r="F6" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="108"/>
+      <c r="G6" s="112"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="112"/>
       <c r="J6" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="K6" s="108"/>
-      <c r="L6" s="108"/>
-      <c r="M6" s="108"/>
+      <c r="K6" s="112"/>
+      <c r="L6" s="112"/>
+      <c r="M6" s="112"/>
     </row>
     <row r="7" spans="1:13" ht="45" customHeight="1">
-      <c r="A7" s="107"/>
+      <c r="A7" s="111"/>
       <c r="B7" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="109"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="111"/>
+      <c r="C7" s="113"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="114"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="115"/>
     </row>
     <row r="9" spans="1:13" ht="39.75" customHeight="1">
       <c r="A9" s="35" t="s">

</xml_diff>

<commit_message>
updated HPI/LPI/LPNI to put all NAs or missing data as TBDs, removed modernization timeline tab, edited text in template.
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2974 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
@@ -9,21 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
     <sheet name="System Overview" sheetId="21" r:id="rId2"/>
     <sheet name="Software Lifecycles" sheetId="22" r:id="rId3"/>
     <sheet name="Hardware Lifecycles" sheetId="23" r:id="rId4"/>
-    <sheet name="Modernization Timeline" sheetId="29" r:id="rId5"/>
-    <sheet name="System Data" sheetId="30" r:id="rId6"/>
-    <sheet name="SOR Overlap With DHMSM" sheetId="28" r:id="rId7"/>
-    <sheet name="DHMSM Data Requirements" sheetId="26" r:id="rId8"/>
-    <sheet name="System Interfaces" sheetId="27" r:id="rId9"/>
-    <sheet name="Summary Charts" sheetId="34" r:id="rId10"/>
+    <sheet name="System Data" sheetId="30" r:id="rId5"/>
+    <sheet name="SOR Overlap With DHMSM" sheetId="28" r:id="rId6"/>
+    <sheet name="DHMSM Data Requirements" sheetId="26" r:id="rId7"/>
+    <sheet name="System Interfaces" sheetId="27" r:id="rId8"/>
+    <sheet name="Summary Charts" sheetId="34" r:id="rId9"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
@@ -34,7 +34,6 @@
     <externalReference r:id="rId18"/>
     <externalReference r:id="rId19"/>
     <externalReference r:id="rId20"/>
-    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="Additional">[1]Data!$D$3:$D$15</definedName>
@@ -63,7 +62,6 @@
     <definedName name="HW">[5]SiteDB2!$L$2:$L$330</definedName>
     <definedName name="I_O" localSheetId="0">#REF!</definedName>
     <definedName name="I_O" localSheetId="4">#REF!</definedName>
-    <definedName name="I_O" localSheetId="5">#REF!</definedName>
     <definedName name="I_O" localSheetId="1">#REF!</definedName>
     <definedName name="I_O">#REF!</definedName>
     <definedName name="Link3">[6]Data1!$D$4:$D$182</definedName>
@@ -76,12 +74,12 @@
     <definedName name="Portal_ROI">[2]BOM!$N$46</definedName>
     <definedName name="Portal_SUM">'[2]POM 2 Enabler - FY12'!$N$102</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'System Overview'!$A$2:$M$11</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="7">'DHMSM Data Requirements'!$6:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="6">'DHMSM Data Requirements'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Hardware Lifecycles'!$9:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Software Lifecycles'!$9:$9</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="6">'SOR Overlap With DHMSM'!$6:$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="5">'System Data'!$6:$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="8">'System Interfaces'!$9:$9</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">'SOR Overlap With DHMSM'!$6:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">'System Data'!$6:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="7">'System Interfaces'!$9:$9</definedName>
     <definedName name="Priority3">[6]Data1!$B$4:$B$6</definedName>
     <definedName name="ProcContractMonths">'[2]New Timeline'!$A$22</definedName>
     <definedName name="RangeBLU">[7]BLUBackEnd!$G$5:$G$49</definedName>
@@ -100,7 +98,6 @@
     <definedName name="Teams">[2]Cheat!$A$38:$A$39</definedName>
     <definedName name="Type" localSheetId="0">#REF!</definedName>
     <definedName name="Type" localSheetId="4">#REF!</definedName>
-    <definedName name="Type" localSheetId="5">#REF!</definedName>
     <definedName name="Type" localSheetId="1">#REF!</definedName>
     <definedName name="Type">#REF!</definedName>
     <definedName name="UDDI_ROI">[2]BOM!$N$58</definedName>
@@ -112,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="88">
   <si>
     <t>Garrison / Theater</t>
   </si>
@@ -222,25 +219,7 @@
     <t>Report Overview</t>
   </si>
   <si>
-    <t>System Modernization Timeline</t>
-  </si>
-  <si>
-    <t>Software Cost</t>
-  </si>
-  <si>
-    <t>Hardware Cost</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>This section displays the current @SYSTEM@ interfaces and how they are affected by DHMSM deployment.</t>
-  </si>
-  <si>
-    <t>Software License Budget</t>
-  </si>
-  <si>
-    <t>Hardware Budget</t>
   </si>
   <si>
     <t>Direct Cost</t>
@@ -317,15 +296,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>Software characteristics are based upon TAP data submissions provided by the DHA and Services program offices. Projected upgrade costs are based solely upon data provided to OTM.</t>
-  </si>
-  <si>
-    <t>Hardware characteristics are based upon TAP data submissions provided by the DHA and Services program offices. Projected upgrade costs are based solely upon data provided to OTM.</t>
-  </si>
-  <si>
-    <t>This section displays the cost to upgrade software and hardware that @SYSTEM@ uses as the modules reach end-of-life.</t>
   </si>
   <si>
     <t>System Maturity</t>
@@ -431,6 +401,12 @@
   <si>
     <t>Proposed Temporary Interfaces with DHMSM - Legacy Consumer</t>
   </si>
+  <si>
+    <t>Software characteristics are based upon TAP data submissions provided by the DHA and Services program offices for each of their systems. Annual software sustainment costs were provided by the system owners as part of their budgets. Projected product upgrade costs are taken from industry pricing where available. This tab is broken down into three points in time (current state, IOC, and FOC for DHMSM) to illustrate the changing lifecycle of the system’s products over time and to more closely detail transition plans as information is made available.</t>
+  </si>
+  <si>
+    <t>Hardware characteristics are based upon TAP data submissions provided by the DHA and Services program offices for each of their systems. Annual hardware sustainment costs were provided by the system owners as part of their budgets. Projected product upgrade costs are taken from industry pricing where available. This tab is broken down into three points in time (current state, IOC, and FOC for DHMSM) to illustrate the changing lifecycle of the system’s products over time and to more closely detail transition plans as information is made available.</t>
+  </si>
 </sst>
 </file>
 
@@ -440,7 +416,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -577,12 +553,6 @@
       <color theme="1"/>
       <name val="Impact"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9.5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -895,7 +865,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -950,14 +920,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="21" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="22" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="21" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -969,12 +933,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -984,10 +948,10 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="48" applyBorder="1"/>
@@ -997,7 +961,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1015,13 +979,13 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1150,9 +1114,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1177,7 +1138,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1475,11 +1436,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="466315792"/>
-        <c:axId val="466315400"/>
+        <c:axId val="471352400"/>
+        <c:axId val="471352792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="466315792"/>
+        <c:axId val="471352400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1489,7 +1450,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="466315400"/>
+        <c:crossAx val="471352792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1497,7 +1458,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="466315400"/>
+        <c:axId val="471352792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1508,7 +1469,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="466315792"/>
+        <c:crossAx val="471352400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1641,11 +1602,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="466315008"/>
-        <c:axId val="497266952"/>
+        <c:axId val="471353576"/>
+        <c:axId val="471353968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="466315008"/>
+        <c:axId val="471353576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1655,7 +1616,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="497266952"/>
+        <c:crossAx val="471353968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1663,7 +1624,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="497266952"/>
+        <c:axId val="471353968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1674,7 +1635,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="466315008"/>
+        <c:crossAx val="471353576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1955,11 +1916,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="497267736"/>
-        <c:axId val="497268128"/>
+        <c:axId val="471354752"/>
+        <c:axId val="403662720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="497267736"/>
+        <c:axId val="471354752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1969,7 +1930,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="497268128"/>
+        <c:crossAx val="403662720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1977,7 +1938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="497268128"/>
+        <c:axId val="403662720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1988,14 +1949,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="497267736"/>
+        <c:crossAx val="471354752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -44531,151 +44491,151 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="31" customWidth="1"/>
-    <col min="2" max="11" width="9.140625" style="31"/>
-    <col min="12" max="12" width="33.28515625" style="31" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="31"/>
+    <col min="1" max="1" width="17.5703125" style="29" customWidth="1"/>
+    <col min="2" max="11" width="9.140625" style="29"/>
+    <col min="12" max="12" width="33.28515625" style="29" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="32.25" customHeight="1">
-      <c r="A2" s="52" t="s">
-        <v>54</v>
+      <c r="A2" s="50" t="s">
+        <v>48</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="281.25" customHeight="1">
-      <c r="A4" s="54" t="s">
-        <v>89</v>
+      <c r="A4" s="52" t="s">
+        <v>80</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="56"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="54"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="30" customFormat="1" ht="29.25" customHeight="1">
+      <c r="A6" s="50" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" s="32" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A6" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="134.25" customHeight="1">
-      <c r="A8" s="57" t="s">
-        <v>57</v>
+      <c r="A8" s="55" t="s">
+        <v>51</v>
       </c>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="58"/>
-      <c r="L8" s="59"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="57"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -44693,181 +44653,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="A1:C25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="38.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="41" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="38"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="41" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="41" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="40">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
@@ -44876,8 +44661,8 @@
   </sheetPr>
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O54" sqref="O54"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54:I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44897,22 +44682,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="261.75" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="68" t="s">
-        <v>88</v>
+      <c r="C2" s="65"/>
+      <c r="D2" s="66" t="s">
+        <v>79</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="70"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="68"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -44931,20 +44716,20 @@
     </row>
     <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
     </row>
     <row r="5" spans="1:13" ht="7.5" customHeight="1">
       <c r="A5" s="5"/>
@@ -44970,22 +44755,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="68" t="s">
-        <v>58</v>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66" t="s">
+        <v>52</v>
       </c>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="70"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="68"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -44996,645 +44781,645 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
-      <c r="L9" s="74"/>
-      <c r="M9" s="75"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="73"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71" t="s">
+      <c r="C10" s="69"/>
+      <c r="D10" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="72"/>
-      <c r="F10" s="71" t="s">
-        <v>45</v>
+      <c r="E10" s="70"/>
+      <c r="F10" s="69" t="s">
+        <v>39</v>
       </c>
-      <c r="G10" s="71"/>
-      <c r="H10" s="85" t="s">
-        <v>46</v>
+      <c r="G10" s="69"/>
+      <c r="H10" s="83" t="s">
+        <v>40</v>
       </c>
-      <c r="I10" s="86"/>
-      <c r="J10" s="71" t="s">
-        <v>47</v>
+      <c r="I10" s="84"/>
+      <c r="J10" s="69" t="s">
+        <v>41</v>
       </c>
-      <c r="K10" s="71"/>
-      <c r="L10" s="71" t="s">
+      <c r="K10" s="69"/>
+      <c r="L10" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="71"/>
+      <c r="M10" s="69"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="65"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="63"/>
     </row>
     <row r="13" spans="1:13" ht="16.5">
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="72"/>
+      <c r="M13" s="73"/>
+    </row>
+    <row r="14" spans="1:13" ht="51" customHeight="1">
+      <c r="B14" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="78"/>
+      <c r="M14" s="79"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="B15" s="80" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="74"/>
-      <c r="M13" s="75"/>
-    </row>
-    <row r="14" spans="1:13" ht="51" customHeight="1">
-      <c r="B14" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="80"/>
-      <c r="K14" s="80"/>
-      <c r="L14" s="80"/>
-      <c r="M14" s="81"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="B15" s="82" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="83"/>
-      <c r="F15" s="83"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="82" t="s">
-        <v>71</v>
-      </c>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="83"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="84"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="81"/>
+      <c r="L15" s="81"/>
+      <c r="M15" s="82"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="44"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="42"/>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="45"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="47"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="45"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="47"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="45"/>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="45"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="47"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="45"/>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="45"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="47"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="45"/>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="45"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="47"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="45"/>
     </row>
     <row r="22" spans="2:13">
-      <c r="B22" s="45"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="47"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="45"/>
     </row>
     <row r="23" spans="2:13">
-      <c r="B23" s="45"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="47"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="45"/>
     </row>
     <row r="24" spans="2:13">
-      <c r="B24" s="45"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="47"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="45"/>
     </row>
     <row r="25" spans="2:13">
-      <c r="B25" s="45"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="47"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="45"/>
     </row>
     <row r="26" spans="2:13">
-      <c r="B26" s="45"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46"/>
-      <c r="L26" s="46"/>
-      <c r="M26" s="47"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="45"/>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="45"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="46"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="47"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="45"/>
     </row>
     <row r="28" spans="2:13">
-      <c r="B28" s="45"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="46"/>
-      <c r="J28" s="46"/>
-      <c r="K28" s="46"/>
-      <c r="L28" s="46"/>
-      <c r="M28" s="47"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="44"/>
+      <c r="M28" s="45"/>
     </row>
     <row r="29" spans="2:13">
-      <c r="B29" s="45"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="47"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="45"/>
     </row>
     <row r="30" spans="2:13">
-      <c r="B30" s="45"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="46"/>
-      <c r="M30" s="47"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="45"/>
     </row>
     <row r="31" spans="2:13">
-      <c r="B31" s="48"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="50"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="48"/>
     </row>
     <row r="33" spans="2:13" ht="16.5">
-      <c r="B33" s="73" t="s">
-        <v>72</v>
+      <c r="B33" s="71" t="s">
+        <v>63</v>
       </c>
-      <c r="C33" s="74"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="75"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="72"/>
+      <c r="F33" s="72"/>
+      <c r="G33" s="72"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="72"/>
+      <c r="K33" s="72"/>
+      <c r="L33" s="72"/>
+      <c r="M33" s="73"/>
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B34" s="76" t="s">
-        <v>78</v>
+      <c r="B34" s="74" t="s">
+        <v>69</v>
       </c>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="77"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="77"/>
-      <c r="L34" s="77"/>
-      <c r="M34" s="78"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="75"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="75"/>
+      <c r="L34" s="75"/>
+      <c r="M34" s="76"/>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="42"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="44"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="41"/>
+      <c r="M35" s="42"/>
     </row>
     <row r="36" spans="2:13">
-      <c r="B36" s="45"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="46"/>
-      <c r="J36" s="46"/>
-      <c r="K36" s="46"/>
-      <c r="L36" s="46"/>
-      <c r="M36" s="47"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
+      <c r="L36" s="44"/>
+      <c r="M36" s="45"/>
     </row>
     <row r="37" spans="2:13">
-      <c r="B37" s="45"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="46"/>
-      <c r="K37" s="46"/>
-      <c r="L37" s="46"/>
-      <c r="M37" s="47"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="45"/>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="45"/>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="46"/>
-      <c r="I38" s="46"/>
-      <c r="J38" s="46"/>
-      <c r="K38" s="46"/>
-      <c r="L38" s="46"/>
-      <c r="M38" s="47"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="44"/>
+      <c r="L38" s="44"/>
+      <c r="M38" s="45"/>
     </row>
     <row r="39" spans="2:13">
-      <c r="B39" s="45"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="46"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="46"/>
-      <c r="J39" s="46"/>
-      <c r="K39" s="46"/>
-      <c r="L39" s="46"/>
-      <c r="M39" s="47"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="45"/>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="45"/>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="46"/>
-      <c r="J40" s="46"/>
-      <c r="K40" s="46"/>
-      <c r="L40" s="46"/>
-      <c r="M40" s="47"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="44"/>
+      <c r="L40" s="44"/>
+      <c r="M40" s="45"/>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="45"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="46"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="46"/>
-      <c r="J41" s="46"/>
-      <c r="K41" s="46"/>
-      <c r="L41" s="46"/>
-      <c r="M41" s="47"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="44"/>
+      <c r="L41" s="44"/>
+      <c r="M41" s="45"/>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="45"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="46"/>
-      <c r="J42" s="46"/>
-      <c r="K42" s="46"/>
-      <c r="L42" s="46"/>
-      <c r="M42" s="47"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="45"/>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="45"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="46"/>
-      <c r="E43" s="46"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="46"/>
-      <c r="H43" s="46"/>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
-      <c r="K43" s="46"/>
-      <c r="L43" s="46"/>
-      <c r="M43" s="47"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="45"/>
     </row>
     <row r="44" spans="2:13">
-      <c r="B44" s="45"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="46"/>
-      <c r="K44" s="46"/>
-      <c r="L44" s="46"/>
-      <c r="M44" s="47"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="44"/>
+      <c r="J44" s="44"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="44"/>
+      <c r="M44" s="45"/>
     </row>
     <row r="45" spans="2:13">
-      <c r="B45" s="45"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
-      <c r="K45" s="46"/>
-      <c r="L45" s="46"/>
-      <c r="M45" s="47"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="44"/>
+      <c r="I45" s="44"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="44"/>
+      <c r="M45" s="45"/>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="45"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="46"/>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
-      <c r="K46" s="46"/>
-      <c r="L46" s="46"/>
-      <c r="M46" s="47"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="44"/>
+      <c r="L46" s="44"/>
+      <c r="M46" s="45"/>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="45"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="46"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="46"/>
-      <c r="G47" s="46"/>
-      <c r="H47" s="46"/>
-      <c r="I47" s="46"/>
-      <c r="J47" s="46"/>
-      <c r="K47" s="46"/>
-      <c r="L47" s="46"/>
-      <c r="M47" s="47"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="44"/>
+      <c r="M47" s="45"/>
     </row>
     <row r="48" spans="2:13">
-      <c r="B48" s="45"/>
-      <c r="C48" s="46"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
-      <c r="F48" s="46"/>
-      <c r="G48" s="46"/>
-      <c r="H48" s="46"/>
-      <c r="I48" s="46"/>
-      <c r="J48" s="46"/>
-      <c r="K48" s="46"/>
-      <c r="L48" s="46"/>
-      <c r="M48" s="47"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="44"/>
+      <c r="L48" s="44"/>
+      <c r="M48" s="45"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="B49" s="45"/>
-      <c r="C49" s="46"/>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="46"/>
-      <c r="G49" s="46"/>
-      <c r="H49" s="46"/>
-      <c r="I49" s="46"/>
-      <c r="J49" s="46"/>
-      <c r="K49" s="46"/>
-      <c r="L49" s="46"/>
-      <c r="M49" s="47"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="44"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="44"/>
+      <c r="J49" s="44"/>
+      <c r="K49" s="44"/>
+      <c r="L49" s="44"/>
+      <c r="M49" s="45"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="B50" s="48"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="49"/>
-      <c r="H50" s="49"/>
-      <c r="I50" s="49"/>
-      <c r="J50" s="49"/>
-      <c r="K50" s="49"/>
-      <c r="L50" s="49"/>
-      <c r="M50" s="50"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="47"/>
+      <c r="I50" s="47"/>
+      <c r="J50" s="47"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="47"/>
+      <c r="M50" s="48"/>
     </row>
     <row r="52" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A52" s="7"/>
-      <c r="B52" s="73" t="s">
-        <v>90</v>
+      <c r="B52" s="71" t="s">
+        <v>81</v>
       </c>
-      <c r="C52" s="74"/>
-      <c r="D52" s="74"/>
-      <c r="E52" s="74"/>
-      <c r="F52" s="74"/>
-      <c r="G52" s="74"/>
-      <c r="H52" s="74"/>
-      <c r="I52" s="74"/>
-      <c r="J52" s="74"/>
-      <c r="K52" s="74"/>
-      <c r="L52" s="74"/>
-      <c r="M52" s="75"/>
+      <c r="C52" s="72"/>
+      <c r="D52" s="72"/>
+      <c r="E52" s="72"/>
+      <c r="F52" s="72"/>
+      <c r="G52" s="72"/>
+      <c r="H52" s="72"/>
+      <c r="I52" s="72"/>
+      <c r="J52" s="72"/>
+      <c r="K52" s="72"/>
+      <c r="L52" s="72"/>
+      <c r="M52" s="73"/>
     </row>
     <row r="53" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A53" s="7"/>
-      <c r="B53" s="60" t="s">
-        <v>92</v>
+      <c r="B53" s="58" t="s">
+        <v>83</v>
       </c>
-      <c r="C53" s="61"/>
-      <c r="D53" s="61"/>
-      <c r="E53" s="62"/>
-      <c r="F53" s="60" t="s">
-        <v>93</v>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="60"/>
+      <c r="F53" s="58" t="s">
+        <v>84</v>
       </c>
-      <c r="G53" s="61"/>
-      <c r="H53" s="61"/>
-      <c r="I53" s="62"/>
-      <c r="J53" s="60" t="s">
-        <v>91</v>
+      <c r="G53" s="59"/>
+      <c r="H53" s="59"/>
+      <c r="I53" s="60"/>
+      <c r="J53" s="58" t="s">
+        <v>82</v>
       </c>
-      <c r="K53" s="61"/>
-      <c r="L53" s="61"/>
-      <c r="M53" s="62"/>
+      <c r="K53" s="59"/>
+      <c r="L53" s="59"/>
+      <c r="M53" s="60"/>
     </row>
     <row r="54" spans="1:13" ht="42.75" customHeight="1">
       <c r="A54" s="5"/>
-      <c r="B54" s="63"/>
-      <c r="C54" s="64"/>
-      <c r="D54" s="64"/>
-      <c r="E54" s="65"/>
-      <c r="F54" s="63"/>
-      <c r="G54" s="64"/>
-      <c r="H54" s="64"/>
-      <c r="I54" s="65"/>
-      <c r="J54" s="63"/>
-      <c r="K54" s="64"/>
-      <c r="L54" s="64"/>
-      <c r="M54" s="65"/>
+      <c r="B54" s="61"/>
+      <c r="C54" s="62"/>
+      <c r="D54" s="62"/>
+      <c r="E54" s="63"/>
+      <c r="F54" s="61"/>
+      <c r="G54" s="62"/>
+      <c r="H54" s="62"/>
+      <c r="I54" s="63"/>
+      <c r="J54" s="61"/>
+      <c r="K54" s="62"/>
+      <c r="L54" s="62"/>
+      <c r="M54" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="31">
@@ -45686,7 +45471,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -45703,90 +45488,90 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="94" t="s">
-        <v>59</v>
+    <row r="5" spans="1:7" ht="68.25" customHeight="1">
+      <c r="A5" s="92" t="s">
+        <v>86</v>
       </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="96"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="94"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="92"/>
-      <c r="C7" s="88" t="s">
-        <v>51</v>
+      <c r="B7" s="90"/>
+      <c r="C7" s="86" t="s">
+        <v>45</v>
       </c>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="90"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="88"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="25.5">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>48</v>
+      <c r="B9" s="33" t="s">
+        <v>42</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="33" t="s">
         <v>22</v>
       </c>
     </row>
@@ -45794,14 +45579,14 @@
       <c r="A10" s="23"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="28"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="28"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -45827,7 +45612,7 @@
   <dimension ref="A2:G10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -45843,71 +45628,71 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="99"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="97"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
     </row>
-    <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="94" t="s">
-        <v>60</v>
+    <row r="5" spans="1:7" ht="67.5" customHeight="1">
+      <c r="A5" s="92" t="s">
+        <v>87</v>
       </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="96"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="94"/>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="93"/>
-      <c r="C7" s="100" t="s">
-        <v>52</v>
+      <c r="B7" s="91"/>
+      <c r="C7" s="98" t="s">
+        <v>46</v>
       </c>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
     </row>
     <row r="9" spans="1:7" ht="25.5">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>48</v>
+      <c r="B9" s="33" t="s">
+        <v>42</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="33" t="s">
         <v>24</v>
       </c>
     </row>
@@ -45915,10 +45700,10 @@
       <c r="A10" s="23"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="28"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="28"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -45940,187 +45725,10 @@
     <tabColor rgb="FF366092"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:J11"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" style="1" customWidth="1"/>
-    <col min="2" max="10" width="15" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="104" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-    </row>
-    <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-    </row>
-    <row r="4" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A4" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="101" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="103"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" ht="24" customHeight="1">
-      <c r="B6" s="35">
-        <v>2015</v>
-      </c>
-      <c r="C6" s="35">
-        <v>2016</v>
-      </c>
-      <c r="D6" s="35">
-        <v>2017</v>
-      </c>
-      <c r="E6" s="35">
-        <v>2018</v>
-      </c>
-      <c r="F6" s="35">
-        <v>2019</v>
-      </c>
-      <c r="G6" s="35">
-        <v>2020</v>
-      </c>
-      <c r="H6" s="35">
-        <v>2021</v>
-      </c>
-      <c r="I6" s="35">
-        <v>2022</v>
-      </c>
-      <c r="J6" s="35" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="41.25" customHeight="1">
-      <c r="A7" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="24">
-        <v>0</v>
-      </c>
-      <c r="C7" s="24">
-        <v>0</v>
-      </c>
-      <c r="D7" s="24">
-        <v>0</v>
-      </c>
-      <c r="E7" s="24">
-        <v>0</v>
-      </c>
-      <c r="F7" s="24">
-        <v>0</v>
-      </c>
-      <c r="G7" s="24">
-        <v>0</v>
-      </c>
-      <c r="H7" s="24">
-        <v>0</v>
-      </c>
-      <c r="I7" s="24">
-        <v>0</v>
-      </c>
-      <c r="J7" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="41.25" customHeight="1">
-      <c r="A8" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="24">
-        <v>0</v>
-      </c>
-      <c r="C8" s="24">
-        <v>0</v>
-      </c>
-      <c r="D8" s="24">
-        <v>0</v>
-      </c>
-      <c r="E8" s="24">
-        <v>0</v>
-      </c>
-      <c r="F8" s="24">
-        <v>0</v>
-      </c>
-      <c r="G8" s="24">
-        <v>0</v>
-      </c>
-      <c r="H8" s="24">
-        <v>0</v>
-      </c>
-      <c r="I8" s="24">
-        <v>0</v>
-      </c>
-      <c r="J8" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="41.25" customHeight="1">
-      <c r="A10" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="41.25" customHeight="1">
-      <c r="A11" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="25">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="A2:J2"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="75" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF366092"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -46133,46 +45741,46 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1"/>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
     </row>
     <row r="4" spans="1:10" ht="53.25" customHeight="1">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="105" t="s">
-        <v>80</v>
+      <c r="B4" s="102" t="s">
+        <v>71</v>
       </c>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="107"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="104"/>
     </row>
     <row r="6" spans="1:10" ht="39.75" customHeight="1">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="35" t="s">
-        <v>53</v>
+      <c r="B6" s="33" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -46185,7 +45793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF366092"/>
@@ -46205,10 +45813,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18">
-      <c r="A2" s="104" t="s">
-        <v>55</v>
+      <c r="A2" s="101" t="s">
+        <v>49</v>
       </c>
-      <c r="B2" s="104"/>
+      <c r="B2" s="101"/>
     </row>
     <row r="3" spans="1:2" ht="18">
       <c r="A3" s="12"/>
@@ -46227,10 +45835,10 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="33" t="s">
         <v>7</v>
       </c>
     </row>
@@ -46248,7 +45856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF366092"/>
@@ -46269,11 +45877,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -46284,10 +45892,10 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="101" t="s">
-        <v>82</v>
+      <c r="B4" s="99" t="s">
+        <v>73</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="100"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -46295,14 +45903,14 @@
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="35" t="s">
-        <v>49</v>
+      <c r="C6" s="33" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -46321,7 +45929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF366092"/>
@@ -46353,114 +45961,114 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1"/>
     <row r="2" spans="1:13" ht="18" customHeight="1">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="104"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
     </row>
     <row r="4" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="117"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="108" t="s">
-        <v>40</v>
+      <c r="B4" s="114"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="105" t="s">
+        <v>36</v>
       </c>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109"/>
-      <c r="M4" s="110"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="106"/>
+      <c r="M4" s="107"/>
     </row>
     <row r="6" spans="1:13" ht="96.75" customHeight="1">
-      <c r="A6" s="111" t="s">
-        <v>83</v>
+      <c r="A6" s="108" t="s">
+        <v>74</v>
       </c>
-      <c r="B6" s="51" t="s">
-        <v>84</v>
+      <c r="B6" s="49" t="s">
+        <v>75</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="51" t="s">
-        <v>86</v>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="49" t="s">
+        <v>77</v>
       </c>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="112"/>
-      <c r="J6" s="51" t="s">
-        <v>87</v>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="49" t="s">
+        <v>78</v>
       </c>
-      <c r="K6" s="112"/>
-      <c r="L6" s="112"/>
-      <c r="M6" s="112"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="109"/>
+      <c r="M6" s="109"/>
     </row>
     <row r="7" spans="1:13" ht="45" customHeight="1">
-      <c r="A7" s="111"/>
-      <c r="B7" s="51" t="s">
-        <v>85</v>
+      <c r="A7" s="108"/>
+      <c r="B7" s="49" t="s">
+        <v>76</v>
       </c>
-      <c r="C7" s="113"/>
-      <c r="D7" s="114"/>
-      <c r="E7" s="114"/>
-      <c r="F7" s="114"/>
-      <c r="G7" s="115"/>
+      <c r="C7" s="110"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="112"/>
     </row>
     <row r="9" spans="1:13" ht="39.75" customHeight="1">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="35" t="s">
+      <c r="H9" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="35" t="s">
+      <c r="I9" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="35" t="s">
+      <c r="J9" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="35" t="s">
-        <v>81</v>
+      <c r="K9" s="33" t="s">
+        <v>72</v>
       </c>
-      <c r="L9" s="36" t="s">
-        <v>43</v>
+      <c r="L9" s="34" t="s">
+        <v>37</v>
       </c>
-      <c r="M9" s="36" t="s">
-        <v>44</v>
+      <c r="M9" s="34" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -46479,11 +46087,11 @@
       <c r="M10" s="22"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="K11" s="27" t="s">
+      <c r="K11" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -46501,4 +46109,179 @@
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="36"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="38">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated transition reports to include HPI and HPNI functionality.
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@3039 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: af3c6274370f62ace2624a87052467c6123bd760
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -352,9 +352,6 @@
     <t>The following graphs provide an overview of the hardware and software maturity for @SYSTEM@, illustrating the number of software and hardware products in each lifecycle phase  at the start of IOC (expected @DATE@).</t>
   </si>
   <si>
-    <t>This section displays the data objects that @SYSTEM@ is a source of record of and the numbers of systems which @SYSTEM@ sends the data to. Additionally, this section displays the data objects that @SYSTEM@ consumes, the other systems that are a source of the data object and the number of low probability systems they provide data for.</t>
-  </si>
-  <si>
     <t>Recommendation</t>
   </si>
   <si>
@@ -406,6 +403,9 @@
   </si>
   <si>
     <t>Hardware characteristics are based upon TAP data submissions provided by the DHA and Services program offices for each of their systems. Annual hardware sustainment costs were provided by the system owners as part of their budgets. Projected product upgrade costs are taken from industry pricing where available. This tab is broken down into three points in time (current state, IOC, and FOC for DHMSM) to illustrate the changing lifecycle of the system’s products over time and to more closely detail transition plans as information is made available.</t>
+  </si>
+  <si>
+    <t>This section displays the data objects that @SYSTEM@ is a source of record of and consumes. For each data object @SYSTEM@ is a source of record of, the number in the @SYSTEM@ column represents the number of systems the data object is passed to. For each data object @SYSTEM@ consumes, the highlighted cells depict the systems @SYSTEM@ receives the data from. The numbers in these cells represent the total number of systems they pass the data objects to.</t>
   </si>
 </sst>
 </file>
@@ -988,45 +988,6 @@
     <xf numFmtId="0" fontId="24" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1054,6 +1015,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1063,11 +1033,41 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1111,12 +1111,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1127,6 +1121,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1436,11 +1436,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="471352400"/>
-        <c:axId val="471352792"/>
+        <c:axId val="531245792"/>
+        <c:axId val="531246184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="471352400"/>
+        <c:axId val="531245792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1450,7 +1450,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="471352792"/>
+        <c:crossAx val="531246184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1458,7 +1458,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="471352792"/>
+        <c:axId val="531246184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1469,7 +1469,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="471352400"/>
+        <c:crossAx val="531245792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1602,11 +1602,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="471353576"/>
-        <c:axId val="471353968"/>
+        <c:axId val="531246968"/>
+        <c:axId val="531247360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="471353576"/>
+        <c:axId val="531246968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1616,7 +1616,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="471353968"/>
+        <c:crossAx val="531247360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1624,7 +1624,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="471353968"/>
+        <c:axId val="531247360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1635,7 +1635,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="471353576"/>
+        <c:crossAx val="531246968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1916,11 +1916,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="471354752"/>
-        <c:axId val="403662720"/>
+        <c:axId val="531248144"/>
+        <c:axId val="531248536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="471354752"/>
+        <c:axId val="531248144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1930,7 +1930,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="403662720"/>
+        <c:crossAx val="531248536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1938,7 +1938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="403662720"/>
+        <c:axId val="531248536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1949,7 +1949,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="471354752"/>
+        <c:crossAx val="531248144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -44485,8 +44485,8 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -44525,7 +44525,7 @@
     </row>
     <row r="4" spans="1:12" ht="281.25" customHeight="1">
       <c r="A4" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="53"/>
       <c r="C4" s="53"/>
@@ -44682,22 +44682,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="261.75" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="66" t="s">
-        <v>79</v>
+      <c r="C2" s="79"/>
+      <c r="D2" s="67" t="s">
+        <v>78</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -44755,22 +44755,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="66" t="s">
+      <c r="C7" s="79"/>
+      <c r="D7" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="69"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -44781,112 +44781,112 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="73"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="60"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69" t="s">
+      <c r="C10" s="73"/>
+      <c r="D10" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="70"/>
-      <c r="F10" s="69" t="s">
+      <c r="E10" s="80"/>
+      <c r="F10" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="69"/>
-      <c r="H10" s="83" t="s">
+      <c r="G10" s="73"/>
+      <c r="H10" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="84"/>
-      <c r="J10" s="69" t="s">
+      <c r="I10" s="75"/>
+      <c r="J10" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69" t="s">
+      <c r="K10" s="73"/>
+      <c r="L10" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="69"/>
+      <c r="M10" s="73"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="63"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="77"/>
     </row>
     <row r="13" spans="1:13" ht="16.5">
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="72"/>
-      <c r="K13" s="72"/>
-      <c r="L13" s="72"/>
-      <c r="M13" s="73"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="60"/>
     </row>
     <row r="14" spans="1:13" ht="51" customHeight="1">
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="79"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="66"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="81"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="80" t="s">
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="81"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="81"/>
-      <c r="L15" s="81"/>
-      <c r="M15" s="82"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="71"/>
+      <c r="M15" s="72"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="40"/>
@@ -45113,36 +45113,36 @@
       <c r="M31" s="48"/>
     </row>
     <row r="33" spans="2:13" ht="16.5">
-      <c r="B33" s="71" t="s">
+      <c r="B33" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="72"/>
-      <c r="K33" s="72"/>
-      <c r="L33" s="72"/>
-      <c r="M33" s="73"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="59"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="59"/>
+      <c r="M33" s="60"/>
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B34" s="74" t="s">
+      <c r="B34" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="75"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="75"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="75"/>
-      <c r="J34" s="75"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="75"/>
-      <c r="M34" s="76"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="62"/>
+      <c r="K34" s="62"/>
+      <c r="L34" s="62"/>
+      <c r="M34" s="63"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="40"/>
@@ -45370,71 +45370,65 @@
     </row>
     <row r="52" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A52" s="7"/>
-      <c r="B52" s="71" t="s">
-        <v>81</v>
+      <c r="B52" s="58" t="s">
+        <v>80</v>
       </c>
-      <c r="C52" s="72"/>
-      <c r="D52" s="72"/>
-      <c r="E52" s="72"/>
-      <c r="F52" s="72"/>
-      <c r="G52" s="72"/>
-      <c r="H52" s="72"/>
-      <c r="I52" s="72"/>
-      <c r="J52" s="72"/>
-      <c r="K52" s="72"/>
-      <c r="L52" s="72"/>
-      <c r="M52" s="73"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="59"/>
+      <c r="F52" s="59"/>
+      <c r="G52" s="59"/>
+      <c r="H52" s="59"/>
+      <c r="I52" s="59"/>
+      <c r="J52" s="59"/>
+      <c r="K52" s="59"/>
+      <c r="L52" s="59"/>
+      <c r="M52" s="60"/>
     </row>
     <row r="53" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A53" s="7"/>
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="81" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="82"/>
+      <c r="D53" s="82"/>
+      <c r="E53" s="83"/>
+      <c r="F53" s="81" t="s">
         <v>83</v>
       </c>
-      <c r="C53" s="59"/>
-      <c r="D53" s="59"/>
-      <c r="E53" s="60"/>
-      <c r="F53" s="58" t="s">
-        <v>84</v>
+      <c r="G53" s="82"/>
+      <c r="H53" s="82"/>
+      <c r="I53" s="83"/>
+      <c r="J53" s="81" t="s">
+        <v>81</v>
       </c>
-      <c r="G53" s="59"/>
-      <c r="H53" s="59"/>
-      <c r="I53" s="60"/>
-      <c r="J53" s="58" t="s">
-        <v>82</v>
-      </c>
-      <c r="K53" s="59"/>
-      <c r="L53" s="59"/>
-      <c r="M53" s="60"/>
+      <c r="K53" s="82"/>
+      <c r="L53" s="82"/>
+      <c r="M53" s="83"/>
     </row>
     <row r="54" spans="1:13" ht="42.75" customHeight="1">
       <c r="A54" s="5"/>
-      <c r="B54" s="61"/>
-      <c r="C54" s="62"/>
-      <c r="D54" s="62"/>
-      <c r="E54" s="63"/>
-      <c r="F54" s="61"/>
-      <c r="G54" s="62"/>
-      <c r="H54" s="62"/>
-      <c r="I54" s="63"/>
-      <c r="J54" s="61"/>
-      <c r="K54" s="62"/>
-      <c r="L54" s="62"/>
-      <c r="M54" s="63"/>
+      <c r="B54" s="76"/>
+      <c r="C54" s="84"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="77"/>
+      <c r="F54" s="76"/>
+      <c r="G54" s="84"/>
+      <c r="H54" s="84"/>
+      <c r="I54" s="77"/>
+      <c r="J54" s="76"/>
+      <c r="K54" s="84"/>
+      <c r="L54" s="84"/>
+      <c r="M54" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B52:M52"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="F54:I54"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -45448,12 +45442,18 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="B52:M52"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45520,7 +45520,7 @@
     </row>
     <row r="5" spans="1:7" ht="68.25" customHeight="1">
       <c r="A5" s="92" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="93"/>
       <c r="C5" s="93"/>
@@ -45651,7 +45651,7 @@
     </row>
     <row r="5" spans="1:7" ht="67.5" customHeight="1">
       <c r="A5" s="92" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="93"/>
       <c r="C5" s="93"/>
@@ -45727,8 +45727,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -45741,34 +45741,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1"/>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
     </row>
     <row r="4" spans="1:10" ht="53.25" customHeight="1">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="102" t="s">
-        <v>71</v>
+      <c r="B4" s="100" t="s">
+        <v>87</v>
       </c>
-      <c r="C4" s="103"/>
-      <c r="D4" s="103"/>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="104"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="102"/>
     </row>
     <row r="6" spans="1:10" ht="39.75" customHeight="1">
       <c r="A6" s="33" t="s">
@@ -45813,10 +45813,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="101"/>
+      <c r="B2" s="99"/>
     </row>
     <row r="3" spans="1:2" ht="18">
       <c r="A3" s="12"/>
@@ -45877,11 +45877,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -45892,10 +45892,10 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="99" t="s">
-        <v>73</v>
+      <c r="B4" s="103" t="s">
+        <v>72</v>
       </c>
-      <c r="C4" s="100"/>
+      <c r="C4" s="104"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -45961,21 +45961,21 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1"/>
     <row r="2" spans="1:13" ht="18" customHeight="1">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
     </row>
     <row r="4" spans="1:13" ht="20.25" customHeight="1">
       <c r="A4" s="113" t="s">
@@ -45998,22 +45998,22 @@
     </row>
     <row r="6" spans="1:13" ht="96.75" customHeight="1">
       <c r="A6" s="108" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="109"/>
       <c r="D6" s="109"/>
       <c r="E6" s="109"/>
       <c r="F6" s="49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G6" s="109"/>
       <c r="H6" s="109"/>
       <c r="I6" s="109"/>
       <c r="J6" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K6" s="109"/>
       <c r="L6" s="109"/>
@@ -46022,7 +46022,7 @@
     <row r="7" spans="1:13" ht="45" customHeight="1">
       <c r="A7" s="108"/>
       <c r="B7" s="49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" s="110"/>
       <c r="D7" s="111"/>
@@ -46062,7 +46062,7 @@
         <v>9</v>
       </c>
       <c r="K9" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L9" s="34" t="s">
         <v>37</v>
@@ -46274,7 +46274,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="38">
         <v>0</v>

</xml_diff>

<commit_message>
updated transition reports to include System BLU sheet
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@3098 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 29877a16f6eb0e000080a9a9e02c428cf537e7a9
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
@@ -17,13 +17,13 @@
     <sheet name="Software Lifecycles" sheetId="22" r:id="rId3"/>
     <sheet name="Hardware Lifecycles" sheetId="23" r:id="rId4"/>
     <sheet name="System Data" sheetId="30" r:id="rId5"/>
-    <sheet name="SOR Overlap With DHMSM" sheetId="28" r:id="rId6"/>
-    <sheet name="DHMSM Data Requirements" sheetId="26" r:id="rId7"/>
-    <sheet name="System Interfaces" sheetId="27" r:id="rId8"/>
-    <sheet name="Summary Charts" sheetId="34" r:id="rId9"/>
+    <sheet name="System BLU" sheetId="35" r:id="rId6"/>
+    <sheet name="SOR Overlap With DHMSM" sheetId="28" r:id="rId7"/>
+    <sheet name="DHMSM Data Requirements" sheetId="26" r:id="rId8"/>
+    <sheet name="System Interfaces" sheetId="27" r:id="rId9"/>
+    <sheet name="Summary Charts" sheetId="34" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
@@ -34,6 +34,7 @@
     <externalReference r:id="rId18"/>
     <externalReference r:id="rId19"/>
     <externalReference r:id="rId20"/>
+    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="Additional">[1]Data!$D$3:$D$15</definedName>
@@ -61,6 +62,7 @@
     <definedName name="HW" localSheetId="0">[4]SiteDB2!$L$2:$L$330</definedName>
     <definedName name="HW">[5]SiteDB2!$L$2:$L$330</definedName>
     <definedName name="I_O" localSheetId="0">#REF!</definedName>
+    <definedName name="I_O" localSheetId="5">#REF!</definedName>
     <definedName name="I_O" localSheetId="4">#REF!</definedName>
     <definedName name="I_O" localSheetId="1">#REF!</definedName>
     <definedName name="I_O">#REF!</definedName>
@@ -74,12 +76,12 @@
     <definedName name="Portal_ROI">[2]BOM!$N$46</definedName>
     <definedName name="Portal_SUM">'[2]POM 2 Enabler - FY12'!$N$102</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'System Overview'!$A$2:$M$11</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="6">'DHMSM Data Requirements'!$6:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="7">'DHMSM Data Requirements'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Hardware Lifecycles'!$9:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Software Lifecycles'!$9:$9</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="5">'SOR Overlap With DHMSM'!$6:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="6">'SOR Overlap With DHMSM'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'System Data'!$6:$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="7">'System Interfaces'!$9:$9</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="8">'System Interfaces'!$9:$9</definedName>
     <definedName name="Priority3">[6]Data1!$B$4:$B$6</definedName>
     <definedName name="ProcContractMonths">'[2]New Timeline'!$A$22</definedName>
     <definedName name="RangeBLU">[7]BLUBackEnd!$G$5:$G$49</definedName>
@@ -97,6 +99,7 @@
     <definedName name="System">'[10]2. System Information'!$D$3</definedName>
     <definedName name="Teams">[2]Cheat!$A$38:$A$39</definedName>
     <definedName name="Type" localSheetId="0">#REF!</definedName>
+    <definedName name="Type" localSheetId="5">#REF!</definedName>
     <definedName name="Type" localSheetId="4">#REF!</definedName>
     <definedName name="Type" localSheetId="1">#REF!</definedName>
     <definedName name="Type">#REF!</definedName>
@@ -109,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="92">
   <si>
     <t>Garrison / Theater</t>
   </si>
@@ -286,15 +289,6 @@
     <t>Contents</t>
   </si>
   <si>
-    <t>This report details the characteristics and modernization activities requried to transition the LPI system to the future-state environment. The report provides the following information and analysis regarding the LPI system:
-1. System Overview
-2. System Hardware and Software Lifecycles
-3. Modernization Timeline
-4. System Data Requirements and Data Provenance
-5. EHR Data Requirements
-6. System Interface Requirements</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -406,6 +400,27 @@
   </si>
   <si>
     <t>This section displays the data objects that @SYSTEM@ is a source of record of and consumes. For each data object @SYSTEM@ is a source of record of, the number in the @SYSTEM@ column represents the number of systems the data object is passed to. For each data object @SYSTEM@ consumes, the highlighted cells depict the systems @SYSTEM@ receives the data from. The numbers in these cells represent the total number of systems they pass the data objects to.</t>
+  </si>
+  <si>
+    <t>System Functionality</t>
+  </si>
+  <si>
+    <t>This section displays the business logic units that @SYSTEM@ provides. Business logic units are defined as automation or system functionality that is provided by @SYSTEM@.</t>
+  </si>
+  <si>
+    <t>Business Logic Unit</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>This report details the characteristics and modernization activities required to transition the HPI system to the future-state environment. The report provides the following information and analysis regarding the HPI system:
+1. System Overview
+2. System Hardware and Software Lifecycles
+3. System Data Requirements and Data Provenance
+4. System Provided Business Logic
+5. EHR Data Requirements
+6. System Interface Requirements</t>
   </si>
 </sst>
 </file>
@@ -865,7 +880,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -964,6 +979,15 @@
     <xf numFmtId="0" fontId="27" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -987,6 +1011,45 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1015,15 +1078,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1033,41 +1087,11 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1436,11 +1460,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="531245792"/>
-        <c:axId val="531246184"/>
+        <c:axId val="450463224"/>
+        <c:axId val="450463616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="531245792"/>
+        <c:axId val="450463224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1450,7 +1474,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="531246184"/>
+        <c:crossAx val="450463616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1458,7 +1482,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="531246184"/>
+        <c:axId val="450463616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1469,7 +1493,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="531245792"/>
+        <c:crossAx val="450463224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1602,11 +1626,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="531246968"/>
-        <c:axId val="531247360"/>
+        <c:axId val="450464400"/>
+        <c:axId val="450464792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="531246968"/>
+        <c:axId val="450464400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1616,7 +1640,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="531247360"/>
+        <c:crossAx val="450464792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1624,7 +1648,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="531247360"/>
+        <c:axId val="450464792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1635,7 +1659,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="531246968"/>
+        <c:crossAx val="450464400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1916,11 +1940,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="531248144"/>
-        <c:axId val="531248536"/>
+        <c:axId val="450465576"/>
+        <c:axId val="450465968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="531248144"/>
+        <c:axId val="450465576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1930,7 +1954,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="531248536"/>
+        <c:crossAx val="450465968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1938,7 +1962,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="531248536"/>
+        <c:axId val="450465968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1949,7 +1973,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="531248144"/>
+        <c:crossAx val="450465576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -44485,8 +44509,8 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:L6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -44503,20 +44527,20 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="32.25" customHeight="1">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -44524,20 +44548,20 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="281.25" customHeight="1">
-      <c r="A4" s="52" t="s">
-        <v>79</v>
+      <c r="A4" s="55" t="s">
+        <v>78</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="54"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="57"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -44545,20 +44569,20 @@
       </c>
     </row>
     <row r="6" spans="1:12" s="30" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -44566,20 +44590,20 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="134.25" customHeight="1">
-      <c r="A8" s="55" t="s">
-        <v>51</v>
+      <c r="A8" s="58" t="s">
+        <v>91</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="57"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="60"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="31"/>
@@ -44653,6 +44677,181 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="36"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="38">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
@@ -44661,7 +44860,7 @@
   </sheetPr>
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F54" sqref="F54:I54"/>
     </sheetView>
   </sheetViews>
@@ -44682,22 +44881,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="261.75" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="67" t="s">
-        <v>78</v>
+      <c r="C2" s="68"/>
+      <c r="D2" s="69" t="s">
+        <v>77</v>
       </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="69"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="71"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -44716,20 +44915,20 @@
     </row>
     <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
     </row>
     <row r="5" spans="1:13" ht="7.5" customHeight="1">
       <c r="A5" s="5"/>
@@ -44755,22 +44954,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="67" t="s">
-        <v>52</v>
+      <c r="C7" s="68"/>
+      <c r="D7" s="69" t="s">
+        <v>51</v>
       </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="69"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="71"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -44781,112 +44980,112 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
-      <c r="M9" s="60"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="76"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73" t="s">
+      <c r="C10" s="72"/>
+      <c r="D10" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="80"/>
-      <c r="F10" s="73" t="s">
+      <c r="E10" s="73"/>
+      <c r="F10" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="73"/>
-      <c r="H10" s="74" t="s">
+      <c r="G10" s="72"/>
+      <c r="H10" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="75"/>
-      <c r="J10" s="73" t="s">
+      <c r="I10" s="87"/>
+      <c r="J10" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73" t="s">
+      <c r="K10" s="72"/>
+      <c r="L10" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="73"/>
+      <c r="M10" s="72"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="76"/>
-      <c r="K11" s="77"/>
-      <c r="L11" s="76"/>
-      <c r="M11" s="77"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="66"/>
     </row>
     <row r="13" spans="1:13" ht="16.5">
-      <c r="B13" s="58" t="s">
-        <v>53</v>
+      <c r="B13" s="74" t="s">
+        <v>52</v>
       </c>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="60"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="76"/>
     </row>
     <row r="14" spans="1:13" ht="51" customHeight="1">
-      <c r="B14" s="64" t="s">
-        <v>70</v>
+      <c r="B14" s="80" t="s">
+        <v>69</v>
       </c>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="66"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="82"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="B15" s="70" t="s">
-        <v>56</v>
+      <c r="B15" s="83" t="s">
+        <v>55</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="70" t="s">
-        <v>62</v>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="83" t="s">
+        <v>61</v>
       </c>
-      <c r="I15" s="71"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="71"/>
-      <c r="L15" s="71"/>
-      <c r="M15" s="72"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="84"/>
+      <c r="K15" s="84"/>
+      <c r="L15" s="84"/>
+      <c r="M15" s="85"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="40"/>
@@ -45113,36 +45312,36 @@
       <c r="M31" s="48"/>
     </row>
     <row r="33" spans="2:13" ht="16.5">
-      <c r="B33" s="58" t="s">
-        <v>63</v>
+      <c r="B33" s="74" t="s">
+        <v>62</v>
       </c>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="59"/>
-      <c r="K33" s="59"/>
-      <c r="L33" s="59"/>
-      <c r="M33" s="60"/>
+      <c r="C33" s="75"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="75"/>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="75"/>
+      <c r="L33" s="75"/>
+      <c r="M33" s="76"/>
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B34" s="61" t="s">
-        <v>69</v>
+      <c r="B34" s="77" t="s">
+        <v>68</v>
       </c>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="62"/>
-      <c r="K34" s="62"/>
-      <c r="L34" s="62"/>
-      <c r="M34" s="63"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="78"/>
+      <c r="H34" s="78"/>
+      <c r="I34" s="78"/>
+      <c r="J34" s="78"/>
+      <c r="K34" s="78"/>
+      <c r="L34" s="78"/>
+      <c r="M34" s="79"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="40"/>
@@ -45370,65 +45569,71 @@
     </row>
     <row r="52" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A52" s="7"/>
-      <c r="B52" s="58" t="s">
-        <v>80</v>
+      <c r="B52" s="74" t="s">
+        <v>79</v>
       </c>
-      <c r="C52" s="59"/>
-      <c r="D52" s="59"/>
-      <c r="E52" s="59"/>
-      <c r="F52" s="59"/>
-      <c r="G52" s="59"/>
-      <c r="H52" s="59"/>
-      <c r="I52" s="59"/>
-      <c r="J52" s="59"/>
-      <c r="K52" s="59"/>
-      <c r="L52" s="59"/>
-      <c r="M52" s="60"/>
+      <c r="C52" s="75"/>
+      <c r="D52" s="75"/>
+      <c r="E52" s="75"/>
+      <c r="F52" s="75"/>
+      <c r="G52" s="75"/>
+      <c r="H52" s="75"/>
+      <c r="I52" s="75"/>
+      <c r="J52" s="75"/>
+      <c r="K52" s="75"/>
+      <c r="L52" s="75"/>
+      <c r="M52" s="76"/>
     </row>
     <row r="53" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A53" s="7"/>
-      <c r="B53" s="81" t="s">
+      <c r="B53" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53" s="62"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="63"/>
+      <c r="F53" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="C53" s="82"/>
-      <c r="D53" s="82"/>
-      <c r="E53" s="83"/>
-      <c r="F53" s="81" t="s">
-        <v>83</v>
+      <c r="G53" s="62"/>
+      <c r="H53" s="62"/>
+      <c r="I53" s="63"/>
+      <c r="J53" s="61" t="s">
+        <v>80</v>
       </c>
-      <c r="G53" s="82"/>
-      <c r="H53" s="82"/>
-      <c r="I53" s="83"/>
-      <c r="J53" s="81" t="s">
-        <v>81</v>
-      </c>
-      <c r="K53" s="82"/>
-      <c r="L53" s="82"/>
-      <c r="M53" s="83"/>
+      <c r="K53" s="62"/>
+      <c r="L53" s="62"/>
+      <c r="M53" s="63"/>
     </row>
     <row r="54" spans="1:13" ht="42.75" customHeight="1">
       <c r="A54" s="5"/>
-      <c r="B54" s="76"/>
-      <c r="C54" s="84"/>
-      <c r="D54" s="84"/>
-      <c r="E54" s="77"/>
-      <c r="F54" s="76"/>
-      <c r="G54" s="84"/>
-      <c r="H54" s="84"/>
-      <c r="I54" s="77"/>
-      <c r="J54" s="76"/>
-      <c r="K54" s="84"/>
-      <c r="L54" s="84"/>
-      <c r="M54" s="77"/>
+      <c r="B54" s="64"/>
+      <c r="C54" s="65"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="66"/>
+      <c r="F54" s="64"/>
+      <c r="G54" s="65"/>
+      <c r="H54" s="65"/>
+      <c r="I54" s="66"/>
+      <c r="J54" s="64"/>
+      <c r="K54" s="65"/>
+      <c r="L54" s="65"/>
+      <c r="M54" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="B52:M52"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -45442,18 +45647,12 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B52:M52"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="F54:I54"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45492,26 +45691,26 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
@@ -45519,15 +45718,15 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="68.25" customHeight="1">
-      <c r="A5" s="92" t="s">
-        <v>85</v>
+      <c r="A5" s="95" t="s">
+        <v>84</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="94"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="97"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
@@ -45535,17 +45734,17 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="90"/>
-      <c r="C7" s="86" t="s">
+      <c r="B7" s="93"/>
+      <c r="C7" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="88"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="91"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
@@ -45628,50 +45827,50 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="100"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
     </row>
     <row r="5" spans="1:7" ht="67.5" customHeight="1">
-      <c r="A5" s="92" t="s">
-        <v>86</v>
+      <c r="A5" s="95" t="s">
+        <v>85</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="94"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="97"/>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="91"/>
-      <c r="C7" s="98" t="s">
+      <c r="B7" s="94"/>
+      <c r="C7" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="98"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
     </row>
     <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="33" t="s">
@@ -45741,34 +45940,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1"/>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
     </row>
     <row r="4" spans="1:10" ht="53.25" customHeight="1">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="100" t="s">
-        <v>87</v>
+      <c r="B4" s="103" t="s">
+        <v>86</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="102"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="105"/>
     </row>
     <row r="6" spans="1:10" ht="39.75" customHeight="1">
       <c r="A6" s="33" t="s">
@@ -45797,6 +45996,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF366092"/>
+  </sheetPr>
+  <dimension ref="A2:J7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" ht="18" customHeight="1">
+      <c r="A2" s="102" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+    </row>
+    <row r="4" spans="1:10" ht="45.75" customHeight="1">
+      <c r="A4" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="103" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="104"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B4:D4"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF366092"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:B7"/>
@@ -45813,10 +46083,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="99"/>
+      <c r="B2" s="102"/>
     </row>
     <row r="3" spans="1:2" ht="18">
       <c r="A3" s="12"/>
@@ -45856,7 +46126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF366092"/>
@@ -45877,11 +46147,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -45892,10 +46162,10 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="103" t="s">
-        <v>72</v>
+      <c r="B4" s="106" t="s">
+        <v>71</v>
       </c>
-      <c r="C4" s="104"/>
+      <c r="C4" s="107"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -45929,7 +46199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF366092"/>
@@ -45961,74 +46231,74 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1"/>
     <row r="2" spans="1:13" ht="18" customHeight="1">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
     </row>
     <row r="4" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="114"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="105" t="s">
+      <c r="B4" s="117"/>
+      <c r="C4" s="118"/>
+      <c r="D4" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="106"/>
-      <c r="L4" s="106"/>
-      <c r="M4" s="107"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="110"/>
     </row>
     <row r="6" spans="1:13" ht="96.75" customHeight="1">
-      <c r="A6" s="108" t="s">
+      <c r="A6" s="111" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="112"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="112"/>
+      <c r="J6" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" s="112"/>
+      <c r="L6" s="112"/>
+      <c r="M6" s="112"/>
+    </row>
+    <row r="7" spans="1:13" ht="45" customHeight="1">
+      <c r="A7" s="111"/>
+      <c r="B7" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="K6" s="109"/>
-      <c r="L6" s="109"/>
-      <c r="M6" s="109"/>
-    </row>
-    <row r="7" spans="1:13" ht="45" customHeight="1">
-      <c r="A7" s="108"/>
-      <c r="B7" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="110"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="112"/>
+      <c r="C7" s="113"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="114"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="115"/>
     </row>
     <row r="9" spans="1:13" ht="39.75" customHeight="1">
       <c r="A9" s="33" t="s">
@@ -46062,7 +46332,7 @@
         <v>9</v>
       </c>
       <c r="K9" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L9" s="34" t="s">
         <v>37</v>
@@ -46109,179 +46379,4 @@
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="A1:C25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="38.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="39" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="36"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="39" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="39" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="38">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated System Interfaces tab legend to reflect future state interface architecture.
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@3214 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmart\workspace64bitNew\SEMOSS_2014\export\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgalbraith\workspace\Semoss\export\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -1012,45 +1012,6 @@
     <xf numFmtId="0" fontId="24" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1078,6 +1039,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1087,11 +1057,41 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1460,11 +1460,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="450463224"/>
-        <c:axId val="450463616"/>
+        <c:axId val="361464304"/>
+        <c:axId val="420109080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="450463224"/>
+        <c:axId val="361464304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1474,7 +1474,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="450463616"/>
+        <c:crossAx val="420109080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1482,7 +1482,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="450463616"/>
+        <c:axId val="420109080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1493,7 +1493,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="450463224"/>
+        <c:crossAx val="361464304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1626,11 +1626,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="450464400"/>
-        <c:axId val="450464792"/>
+        <c:axId val="420109864"/>
+        <c:axId val="420110256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="450464400"/>
+        <c:axId val="420109864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,7 +1640,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="450464792"/>
+        <c:crossAx val="420110256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1648,7 +1648,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="450464792"/>
+        <c:axId val="420110256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1659,7 +1659,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="450464400"/>
+        <c:crossAx val="420109864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1940,11 +1940,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="450465576"/>
-        <c:axId val="450465968"/>
+        <c:axId val="419153440"/>
+        <c:axId val="419153832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="450465576"/>
+        <c:axId val="419153440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1954,7 +1954,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="450465968"/>
+        <c:crossAx val="419153832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1962,7 +1962,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="450465968"/>
+        <c:axId val="419153832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1973,7 +1973,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="450465576"/>
+        <c:crossAx val="419153440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2208,44 +2208,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>70068</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>547921</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Picture 24"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1885950" y="2324100"/>
-          <a:ext cx="6623268" cy="490771"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
@@ -2264,7 +2226,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2273,6 +2235,44 @@
         <a:xfrm>
           <a:off x="1733550" y="1266825"/>
           <a:ext cx="2286198" cy="793768"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>541237</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1819275" y="2305050"/>
+          <a:ext cx="6705600" cy="503137"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -44509,7 +44509,7 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
@@ -44881,22 +44881,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="261.75" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="69" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="72"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -44954,22 +44954,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="69" t="s">
+      <c r="C7" s="82"/>
+      <c r="D7" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="70"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="72"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -44980,112 +44980,112 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="76"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="63"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72" t="s">
+      <c r="C10" s="76"/>
+      <c r="D10" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="72" t="s">
+      <c r="E10" s="83"/>
+      <c r="F10" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="72"/>
-      <c r="H10" s="86" t="s">
+      <c r="G10" s="76"/>
+      <c r="H10" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="87"/>
-      <c r="J10" s="72" t="s">
+      <c r="I10" s="78"/>
+      <c r="J10" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72" t="s">
+      <c r="K10" s="76"/>
+      <c r="L10" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="72"/>
+      <c r="M10" s="76"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="66"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="80"/>
     </row>
     <row r="13" spans="1:13" ht="16.5">
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="75"/>
-      <c r="L13" s="75"/>
-      <c r="M13" s="76"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="63"/>
     </row>
     <row r="14" spans="1:13" ht="51" customHeight="1">
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="81"/>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="82"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="68"/>
+      <c r="M14" s="69"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="B15" s="83" t="s">
+      <c r="B15" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="83" t="s">
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="84"/>
-      <c r="L15" s="84"/>
-      <c r="M15" s="85"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="74"/>
+      <c r="M15" s="75"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="40"/>
@@ -45312,36 +45312,36 @@
       <c r="M31" s="48"/>
     </row>
     <row r="33" spans="2:13" ht="16.5">
-      <c r="B33" s="74" t="s">
+      <c r="B33" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="75"/>
-      <c r="I33" s="75"/>
-      <c r="J33" s="75"/>
-      <c r="K33" s="75"/>
-      <c r="L33" s="75"/>
-      <c r="M33" s="76"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="62"/>
+      <c r="K33" s="62"/>
+      <c r="L33" s="62"/>
+      <c r="M33" s="63"/>
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B34" s="77" t="s">
+      <c r="B34" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
-      <c r="J34" s="78"/>
-      <c r="K34" s="78"/>
-      <c r="L34" s="78"/>
-      <c r="M34" s="79"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
+      <c r="L34" s="65"/>
+      <c r="M34" s="66"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="40"/>
@@ -45569,71 +45569,65 @@
     </row>
     <row r="52" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A52" s="7"/>
-      <c r="B52" s="74" t="s">
+      <c r="B52" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="75"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="75"/>
-      <c r="G52" s="75"/>
-      <c r="H52" s="75"/>
-      <c r="I52" s="75"/>
-      <c r="J52" s="75"/>
-      <c r="K52" s="75"/>
-      <c r="L52" s="75"/>
-      <c r="M52" s="76"/>
+      <c r="C52" s="62"/>
+      <c r="D52" s="62"/>
+      <c r="E52" s="62"/>
+      <c r="F52" s="62"/>
+      <c r="G52" s="62"/>
+      <c r="H52" s="62"/>
+      <c r="I52" s="62"/>
+      <c r="J52" s="62"/>
+      <c r="K52" s="62"/>
+      <c r="L52" s="62"/>
+      <c r="M52" s="63"/>
     </row>
     <row r="53" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A53" s="7"/>
-      <c r="B53" s="61" t="s">
+      <c r="B53" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="62"/>
-      <c r="D53" s="62"/>
-      <c r="E53" s="63"/>
-      <c r="F53" s="61" t="s">
+      <c r="C53" s="85"/>
+      <c r="D53" s="85"/>
+      <c r="E53" s="86"/>
+      <c r="F53" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="G53" s="62"/>
-      <c r="H53" s="62"/>
-      <c r="I53" s="63"/>
-      <c r="J53" s="61" t="s">
+      <c r="G53" s="85"/>
+      <c r="H53" s="85"/>
+      <c r="I53" s="86"/>
+      <c r="J53" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="K53" s="62"/>
-      <c r="L53" s="62"/>
-      <c r="M53" s="63"/>
+      <c r="K53" s="85"/>
+      <c r="L53" s="85"/>
+      <c r="M53" s="86"/>
     </row>
     <row r="54" spans="1:13" ht="42.75" customHeight="1">
       <c r="A54" s="5"/>
-      <c r="B54" s="64"/>
-      <c r="C54" s="65"/>
-      <c r="D54" s="65"/>
-      <c r="E54" s="66"/>
-      <c r="F54" s="64"/>
-      <c r="G54" s="65"/>
-      <c r="H54" s="65"/>
-      <c r="I54" s="66"/>
-      <c r="J54" s="64"/>
-      <c r="K54" s="65"/>
-      <c r="L54" s="65"/>
-      <c r="M54" s="66"/>
+      <c r="B54" s="79"/>
+      <c r="C54" s="87"/>
+      <c r="D54" s="87"/>
+      <c r="E54" s="80"/>
+      <c r="F54" s="79"/>
+      <c r="G54" s="87"/>
+      <c r="H54" s="87"/>
+      <c r="I54" s="80"/>
+      <c r="J54" s="79"/>
+      <c r="K54" s="87"/>
+      <c r="L54" s="87"/>
+      <c r="M54" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B52:M52"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="F54:I54"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -45647,12 +45641,18 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="B52:M52"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -46207,7 +46207,7 @@
   </sheetPr>
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated to reflect new reporting needs for DHSS and DHCS program reviews.
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@3344 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -19,11 +19,11 @@
     <sheet name="System Data" sheetId="30" r:id="rId5"/>
     <sheet name="System BLU" sheetId="35" r:id="rId6"/>
     <sheet name="SOR Overlap With DHMSM" sheetId="28" r:id="rId7"/>
-    <sheet name="DHMSM Data Requirements" sheetId="26" r:id="rId8"/>
-    <sheet name="System Interfaces" sheetId="27" r:id="rId9"/>
-    <sheet name="Summary Charts" sheetId="34" r:id="rId10"/>
+    <sheet name="System Interfaces" sheetId="27" r:id="rId8"/>
+    <sheet name="Summary Charts" sheetId="34" r:id="rId9"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
@@ -34,7 +34,6 @@
     <externalReference r:id="rId18"/>
     <externalReference r:id="rId19"/>
     <externalReference r:id="rId20"/>
-    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="Additional">[1]Data!$D$3:$D$15</definedName>
@@ -76,12 +75,11 @@
     <definedName name="Portal_ROI">[2]BOM!$N$46</definedName>
     <definedName name="Portal_SUM">'[2]POM 2 Enabler - FY12'!$N$102</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'System Overview'!$A$2:$M$11</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="7">'DHMSM Data Requirements'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Hardware Lifecycles'!$9:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Software Lifecycles'!$9:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">'SOR Overlap With DHMSM'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'System Data'!$6:$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="8">'System Interfaces'!$9:$9</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="7">'System Interfaces'!$9:$9</definedName>
     <definedName name="Priority3">[6]Data1!$B$4:$B$6</definedName>
     <definedName name="ProcContractMonths">'[2]New Timeline'!$A$22</definedName>
     <definedName name="RangeBLU">[7]BLUBackEnd!$G$5:$G$49</definedName>
@@ -112,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="88">
   <si>
     <t>Garrison / Theater</t>
   </si>
@@ -136,9 +134,6 @@
   </si>
   <si>
     <t>DHMSM SOR?</t>
-  </si>
-  <si>
-    <t>Capability</t>
   </si>
   <si>
     <t>Services</t>
@@ -207,9 +202,6 @@
     <t>System Data</t>
   </si>
   <si>
-    <t>DHMSM Data Requirements</t>
-  </si>
-  <si>
     <t>System Interfaces</t>
   </si>
   <si>
@@ -243,9 +235,6 @@
     <t>End of Support Date</t>
   </si>
   <si>
-    <t>System Source of Record Business Rule</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -275,9 +264,6 @@
       </rPr>
       <t>(expected @DATE@)</t>
     </r>
-  </si>
-  <si>
-    <t>Provided or Consumed</t>
   </si>
   <si>
     <t>Background</t>
@@ -349,9 +335,6 @@
     <t>Recommendation</t>
   </si>
   <si>
-    <t xml:space="preserve">This section displays the data objects that @SYSTEM@ is the source of record for and that the DHMSM capability will be required to consume. </t>
-  </si>
-  <si>
     <t>Legend</t>
   </si>
   <si>
@@ -399,9 +382,6 @@
     <t>Hardware characteristics are based upon TAP data submissions provided by the DHA and Services program offices for each of their systems. Annual hardware sustainment costs were provided by the system owners as part of their budgets. Projected product upgrade costs are taken from industry pricing where available. This tab is broken down into three points in time (current state, IOC, and FOC for DHMSM) to illustrate the changing lifecycle of the system’s products over time and to more closely detail transition plans as information is made available.</t>
   </si>
   <si>
-    <t>This section displays the data objects that @SYSTEM@ is a source of record of and consumes. For each data object @SYSTEM@ is a source of record of, the number in the @SYSTEM@ column represents the number of systems the data object is passed to. For each data object @SYSTEM@ consumes, the highlighted cells depict the systems @SYSTEM@ receives the data from. The numbers in these cells represent the total number of systems they pass the data objects to.</t>
-  </si>
-  <si>
     <t>System Functionality</t>
   </si>
   <si>
@@ -421,6 +401,12 @@
 4. System Provided Business Logic
 5. EHR Data Requirements
 6. System Interface Requirements</t>
+  </si>
+  <si>
+    <t>This section displays the data objects that @SYSTEM@ creates, reads, or modifies. This information is used in concert with the @SYSTEM@ interface control documents to define what data @SYSTEM is a source of record of and what data @SYSTEM@ consumes.</t>
+  </si>
+  <si>
+    <t>C/R/M</t>
   </si>
 </sst>
 </file>
@@ -880,7 +866,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -960,9 +946,6 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -988,6 +971,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1011,6 +997,45 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1039,15 +1064,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1057,41 +1073,11 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1145,12 +1131,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1460,11 +1440,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="361464304"/>
-        <c:axId val="420109080"/>
+        <c:axId val="419586000"/>
+        <c:axId val="419586392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="361464304"/>
+        <c:axId val="419586000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1474,7 +1454,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="420109080"/>
+        <c:crossAx val="419586392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1482,7 +1462,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="420109080"/>
+        <c:axId val="419586392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1493,7 +1473,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="361464304"/>
+        <c:crossAx val="419586000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1626,11 +1606,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="420109864"/>
-        <c:axId val="420110256"/>
+        <c:axId val="419587176"/>
+        <c:axId val="419587568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="420109864"/>
+        <c:axId val="419587176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,7 +1620,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="420110256"/>
+        <c:crossAx val="419587568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1648,7 +1628,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="420110256"/>
+        <c:axId val="419587568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1659,7 +1639,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="420109864"/>
+        <c:crossAx val="419587176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1940,11 +1920,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="419153440"/>
-        <c:axId val="419153832"/>
+        <c:axId val="419588352"/>
+        <c:axId val="419588744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="419153440"/>
+        <c:axId val="419588352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1954,7 +1934,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="419153832"/>
+        <c:crossAx val="419588744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1962,7 +1942,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="419153832"/>
+        <c:axId val="419588744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1973,7 +1953,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="419153440"/>
+        <c:crossAx val="419588352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -44523,12 +44503,12 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="32.25" customHeight="1">
       <c r="A2" s="53" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B2" s="54"/>
       <c r="C2" s="54"/>
@@ -44544,12 +44524,12 @@
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="281.25" customHeight="1">
       <c r="A4" s="55" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
@@ -44565,12 +44545,12 @@
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="30" customFormat="1" ht="29.25" customHeight="1">
       <c r="A6" s="53" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B6" s="54"/>
       <c r="C6" s="54"/>
@@ -44586,12 +44566,12 @@
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="134.25" customHeight="1">
       <c r="A8" s="58" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -44677,181 +44657,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="A1:C25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="38.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="39" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="36"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="39" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="39" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="38">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
@@ -44881,22 +44686,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="261.75" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="81" t="s">
-        <v>35</v>
+      <c r="B2" s="67" t="s">
+        <v>33</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="70" t="s">
-        <v>77</v>
+      <c r="C2" s="68"/>
+      <c r="D2" s="69" t="s">
+        <v>72</v>
       </c>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="72"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="71"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -44916,7 +44721,7 @@
     <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="53" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="54"/>
       <c r="D4" s="54"/>
@@ -44954,22 +44759,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="81" t="s">
-        <v>29</v>
+      <c r="B7" s="67" t="s">
+        <v>28</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="70" t="s">
-        <v>51</v>
+      <c r="C7" s="68"/>
+      <c r="D7" s="69" t="s">
+        <v>47</v>
       </c>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="72"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="71"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -44980,654 +44785,660 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="63"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="76"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="76" t="s">
+      <c r="B10" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76" t="s">
+      <c r="C10" s="72"/>
+      <c r="D10" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="83"/>
-      <c r="F10" s="76" t="s">
+      <c r="E10" s="73"/>
+      <c r="F10" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="72"/>
+      <c r="H10" s="86" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="87"/>
+      <c r="J10" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="76"/>
-      <c r="H10" s="77" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="78"/>
-      <c r="J10" s="76" t="s">
-        <v>41</v>
-      </c>
-      <c r="K10" s="76"/>
-      <c r="L10" s="76" t="s">
+      <c r="K10" s="72"/>
+      <c r="L10" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="76"/>
+      <c r="M10" s="72"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="79"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="80"/>
-      <c r="L11" s="79"/>
-      <c r="M11" s="80"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="66"/>
     </row>
     <row r="13" spans="1:13" ht="16.5">
-      <c r="B13" s="61" t="s">
-        <v>52</v>
+      <c r="B13" s="74" t="s">
+        <v>48</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="63"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="76"/>
     </row>
     <row r="14" spans="1:13" ht="51" customHeight="1">
-      <c r="B14" s="67" t="s">
-        <v>69</v>
+      <c r="B14" s="80" t="s">
+        <v>65</v>
       </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="68"/>
-      <c r="M14" s="69"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="82"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="B15" s="73" t="s">
-        <v>55</v>
+      <c r="B15" s="83" t="s">
+        <v>51</v>
       </c>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="73" t="s">
-        <v>61</v>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="83" t="s">
+        <v>57</v>
       </c>
-      <c r="I15" s="74"/>
-      <c r="J15" s="74"/>
-      <c r="K15" s="74"/>
-      <c r="L15" s="74"/>
-      <c r="M15" s="75"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="84"/>
+      <c r="K15" s="84"/>
+      <c r="L15" s="84"/>
+      <c r="M15" s="85"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="B16" s="40"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="42"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="41"/>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="43"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="45"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="44"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="43"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="45"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="44"/>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="45"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="44"/>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="43"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="45"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="44"/>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="43"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="45"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="44"/>
     </row>
     <row r="22" spans="2:13">
-      <c r="B22" s="43"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="45"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="44"/>
     </row>
     <row r="23" spans="2:13">
-      <c r="B23" s="43"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="45"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="44"/>
     </row>
     <row r="24" spans="2:13">
-      <c r="B24" s="43"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="45"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="44"/>
     </row>
     <row r="25" spans="2:13">
-      <c r="B25" s="43"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="45"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="44"/>
     </row>
     <row r="26" spans="2:13">
-      <c r="B26" s="43"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="44"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="45"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="44"/>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="43"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="45"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="44"/>
     </row>
     <row r="28" spans="2:13">
-      <c r="B28" s="43"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="45"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="44"/>
     </row>
     <row r="29" spans="2:13">
-      <c r="B29" s="43"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="45"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="44"/>
     </row>
     <row r="30" spans="2:13">
-      <c r="B30" s="43"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="44"/>
-      <c r="L30" s="44"/>
-      <c r="M30" s="45"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="44"/>
     </row>
     <row r="31" spans="2:13">
-      <c r="B31" s="46"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="47"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="48"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="47"/>
     </row>
     <row r="33" spans="2:13" ht="16.5">
-      <c r="B33" s="61" t="s">
-        <v>62</v>
+      <c r="B33" s="74" t="s">
+        <v>58</v>
       </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="62"/>
-      <c r="H33" s="62"/>
-      <c r="I33" s="62"/>
-      <c r="J33" s="62"/>
-      <c r="K33" s="62"/>
-      <c r="L33" s="62"/>
-      <c r="M33" s="63"/>
+      <c r="C33" s="75"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="75"/>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="75"/>
+      <c r="L33" s="75"/>
+      <c r="M33" s="76"/>
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B34" s="64" t="s">
-        <v>68</v>
+      <c r="B34" s="77" t="s">
+        <v>64</v>
       </c>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="65"/>
-      <c r="L34" s="65"/>
-      <c r="M34" s="66"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="78"/>
+      <c r="H34" s="78"/>
+      <c r="I34" s="78"/>
+      <c r="J34" s="78"/>
+      <c r="K34" s="78"/>
+      <c r="L34" s="78"/>
+      <c r="M34" s="79"/>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="40"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
-      <c r="J35" s="41"/>
-      <c r="K35" s="41"/>
-      <c r="L35" s="41"/>
-      <c r="M35" s="42"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="40"/>
+      <c r="L35" s="40"/>
+      <c r="M35" s="41"/>
     </row>
     <row r="36" spans="2:13">
-      <c r="B36" s="43"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="44"/>
-      <c r="M36" s="45"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="44"/>
     </row>
     <row r="37" spans="2:13">
-      <c r="B37" s="43"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="44"/>
-      <c r="L37" s="44"/>
-      <c r="M37" s="45"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="43"/>
+      <c r="M37" s="44"/>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="43"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="44"/>
-      <c r="K38" s="44"/>
-      <c r="L38" s="44"/>
-      <c r="M38" s="45"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="43"/>
+      <c r="M38" s="44"/>
     </row>
     <row r="39" spans="2:13">
-      <c r="B39" s="43"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="44"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="44"/>
-      <c r="K39" s="44"/>
-      <c r="L39" s="44"/>
-      <c r="M39" s="45"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="43"/>
+      <c r="M39" s="44"/>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="43"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="44"/>
-      <c r="M40" s="45"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="43"/>
+      <c r="L40" s="43"/>
+      <c r="M40" s="44"/>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="43"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="44"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="44"/>
-      <c r="J41" s="44"/>
-      <c r="K41" s="44"/>
-      <c r="L41" s="44"/>
-      <c r="M41" s="45"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="43"/>
+      <c r="M41" s="44"/>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="43"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44"/>
-      <c r="K42" s="44"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="45"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="43"/>
+      <c r="M42" s="44"/>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="43"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="45"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="43"/>
+      <c r="M43" s="44"/>
     </row>
     <row r="44" spans="2:13">
-      <c r="B44" s="43"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="44"/>
-      <c r="L44" s="44"/>
-      <c r="M44" s="45"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="43"/>
+      <c r="M44" s="44"/>
     </row>
     <row r="45" spans="2:13">
-      <c r="B45" s="43"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="44"/>
-      <c r="L45" s="44"/>
-      <c r="M45" s="45"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="43"/>
+      <c r="M45" s="44"/>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="43"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
-      <c r="K46" s="44"/>
-      <c r="L46" s="44"/>
-      <c r="M46" s="45"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="43"/>
+      <c r="M46" s="44"/>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="43"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="44"/>
-      <c r="H47" s="44"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
-      <c r="K47" s="44"/>
-      <c r="L47" s="44"/>
-      <c r="M47" s="45"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="43"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="43"/>
+      <c r="M47" s="44"/>
     </row>
     <row r="48" spans="2:13">
-      <c r="B48" s="43"/>
-      <c r="C48" s="44"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="44"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="44"/>
-      <c r="K48" s="44"/>
-      <c r="L48" s="44"/>
-      <c r="M48" s="45"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="43"/>
+      <c r="M48" s="44"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="B49" s="43"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="44"/>
-      <c r="E49" s="44"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="44"/>
-      <c r="H49" s="44"/>
-      <c r="I49" s="44"/>
-      <c r="J49" s="44"/>
-      <c r="K49" s="44"/>
-      <c r="L49" s="44"/>
-      <c r="M49" s="45"/>
+      <c r="B49" s="42"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="43"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43"/>
+      <c r="I49" s="43"/>
+      <c r="J49" s="43"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="43"/>
+      <c r="M49" s="44"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="B50" s="46"/>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
-      <c r="H50" s="47"/>
-      <c r="I50" s="47"/>
-      <c r="J50" s="47"/>
-      <c r="K50" s="47"/>
-      <c r="L50" s="47"/>
-      <c r="M50" s="48"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="46"/>
+      <c r="M50" s="47"/>
     </row>
     <row r="52" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A52" s="7"/>
-      <c r="B52" s="61" t="s">
-        <v>79</v>
+      <c r="B52" s="74" t="s">
+        <v>74</v>
       </c>
-      <c r="C52" s="62"/>
-      <c r="D52" s="62"/>
-      <c r="E52" s="62"/>
-      <c r="F52" s="62"/>
-      <c r="G52" s="62"/>
-      <c r="H52" s="62"/>
-      <c r="I52" s="62"/>
-      <c r="J52" s="62"/>
-      <c r="K52" s="62"/>
-      <c r="L52" s="62"/>
-      <c r="M52" s="63"/>
+      <c r="C52" s="75"/>
+      <c r="D52" s="75"/>
+      <c r="E52" s="75"/>
+      <c r="F52" s="75"/>
+      <c r="G52" s="75"/>
+      <c r="H52" s="75"/>
+      <c r="I52" s="75"/>
+      <c r="J52" s="75"/>
+      <c r="K52" s="75"/>
+      <c r="L52" s="75"/>
+      <c r="M52" s="76"/>
     </row>
     <row r="53" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A53" s="7"/>
-      <c r="B53" s="84" t="s">
-        <v>81</v>
+      <c r="B53" s="61" t="s">
+        <v>76</v>
       </c>
-      <c r="C53" s="85"/>
-      <c r="D53" s="85"/>
-      <c r="E53" s="86"/>
-      <c r="F53" s="84" t="s">
-        <v>82</v>
+      <c r="C53" s="62"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="63"/>
+      <c r="F53" s="61" t="s">
+        <v>77</v>
       </c>
-      <c r="G53" s="85"/>
-      <c r="H53" s="85"/>
-      <c r="I53" s="86"/>
-      <c r="J53" s="84" t="s">
-        <v>80</v>
+      <c r="G53" s="62"/>
+      <c r="H53" s="62"/>
+      <c r="I53" s="63"/>
+      <c r="J53" s="61" t="s">
+        <v>75</v>
       </c>
-      <c r="K53" s="85"/>
-      <c r="L53" s="85"/>
-      <c r="M53" s="86"/>
+      <c r="K53" s="62"/>
+      <c r="L53" s="62"/>
+      <c r="M53" s="63"/>
     </row>
     <row r="54" spans="1:13" ht="42.75" customHeight="1">
       <c r="A54" s="5"/>
-      <c r="B54" s="79"/>
-      <c r="C54" s="87"/>
-      <c r="D54" s="87"/>
-      <c r="E54" s="80"/>
-      <c r="F54" s="79"/>
-      <c r="G54" s="87"/>
-      <c r="H54" s="87"/>
-      <c r="I54" s="80"/>
-      <c r="J54" s="79"/>
-      <c r="K54" s="87"/>
-      <c r="L54" s="87"/>
-      <c r="M54" s="80"/>
+      <c r="B54" s="64"/>
+      <c r="C54" s="65"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="66"/>
+      <c r="F54" s="64"/>
+      <c r="G54" s="65"/>
+      <c r="H54" s="65"/>
+      <c r="I54" s="66"/>
+      <c r="J54" s="64"/>
+      <c r="K54" s="65"/>
+      <c r="L54" s="65"/>
+      <c r="M54" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="B52:M52"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -45641,18 +45452,12 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B52:M52"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="F54:I54"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45687,12 +45492,12 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
       <c r="A2" s="88" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="88"/>
       <c r="C2" s="88"/>
@@ -45703,7 +45508,7 @@
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
       <c r="A3" s="94" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="94"/>
       <c r="C3" s="94"/>
@@ -45714,12 +45519,12 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="68.25" customHeight="1">
       <c r="A5" s="95" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B5" s="96"/>
       <c r="C5" s="96"/>
@@ -45730,16 +45535,16 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
       <c r="A7" s="92" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="93"/>
       <c r="C7" s="89" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7" s="90"/>
       <c r="E7" s="90"/>
@@ -45748,30 +45553,30 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="33" t="s">
+      <c r="E9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="F9" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="33" t="s">
-        <v>19</v>
-      </c>
       <c r="G9" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -45785,7 +45590,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -45828,7 +45633,7 @@
   <sheetData>
     <row r="2" spans="1:7" ht="18" customHeight="1">
       <c r="A2" s="98" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="99"/>
       <c r="C2" s="99"/>
@@ -45850,7 +45655,7 @@
     </row>
     <row r="5" spans="1:7" ht="67.5" customHeight="1">
       <c r="A5" s="95" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B5" s="96"/>
       <c r="C5" s="96"/>
@@ -45861,11 +45666,11 @@
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
       <c r="A7" s="94" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="94"/>
       <c r="C7" s="101" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D7" s="101"/>
       <c r="E7" s="101"/>
@@ -45874,25 +45679,25 @@
     </row>
     <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="F9" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="33" t="s">
-        <v>19</v>
-      </c>
       <c r="G9" s="33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -45927,7 +45732,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection sqref="A1:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -45941,7 +45746,7 @@
     <row r="1" spans="1:10" ht="18" customHeight="1"/>
     <row r="2" spans="1:10" ht="18" customHeight="1">
       <c r="A2" s="102" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="102"/>
       <c r="C2" s="102"/>
@@ -45954,7 +45759,7 @@
       <c r="J2" s="102"/>
     </row>
     <row r="4" spans="1:10" ht="53.25" customHeight="1">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="52" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="103" t="s">
@@ -45974,7 +45779,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -46013,40 +45818,40 @@
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
       <c r="A2" s="102" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B2" s="102"/>
       <c r="C2" s="102"/>
       <c r="D2" s="102"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="4" spans="1:10" ht="45.75" customHeight="1">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="49" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="103" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C4" s="104"/>
       <c r="D4" s="105"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="33" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -46084,7 +45889,7 @@
   <sheetData>
     <row r="2" spans="1:2" ht="18">
       <c r="A2" s="102" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B2" s="102"/>
     </row>
@@ -46097,7 +45902,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -46132,79 +45937,6 @@
     <tabColor rgb="FF366092"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:C7"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="23" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24" style="1" customWidth="1"/>
-    <col min="3" max="3" width="67.28515625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="102" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-    </row>
-    <row r="3" spans="1:3" ht="18">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-    </row>
-    <row r="4" spans="1:3" ht="25.5" customHeight="1">
-      <c r="A4" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="106" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="107"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B4:C4"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="78" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF366092"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
@@ -46232,7 +45964,7 @@
     <row r="1" spans="1:13" ht="18" customHeight="1"/>
     <row r="2" spans="1:13" ht="18" customHeight="1">
       <c r="A2" s="102" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="102"/>
       <c r="C2" s="102"/>
@@ -46248,97 +45980,97 @@
       <c r="M2" s="102"/>
     </row>
     <row r="4" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="117"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="108" t="s">
-        <v>36</v>
+      <c r="B4" s="115"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="106" t="s">
+        <v>34</v>
       </c>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109"/>
-      <c r="M4" s="110"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="107"/>
+      <c r="M4" s="108"/>
     </row>
     <row r="6" spans="1:13" ht="96.75" customHeight="1">
-      <c r="A6" s="111" t="s">
-        <v>72</v>
+      <c r="A6" s="109" t="s">
+        <v>67</v>
       </c>
-      <c r="B6" s="49" t="s">
-        <v>73</v>
+      <c r="B6" s="48" t="s">
+        <v>68</v>
       </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="49" t="s">
-        <v>75</v>
+      <c r="C6" s="110"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="48" t="s">
+        <v>70</v>
       </c>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="112"/>
-      <c r="J6" s="49" t="s">
-        <v>76</v>
+      <c r="G6" s="110"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="110"/>
+      <c r="J6" s="48" t="s">
+        <v>71</v>
       </c>
-      <c r="K6" s="112"/>
-      <c r="L6" s="112"/>
-      <c r="M6" s="112"/>
+      <c r="K6" s="110"/>
+      <c r="L6" s="110"/>
+      <c r="M6" s="110"/>
     </row>
     <row r="7" spans="1:13" ht="45" customHeight="1">
-      <c r="A7" s="111"/>
-      <c r="B7" s="49" t="s">
-        <v>74</v>
+      <c r="A7" s="109"/>
+      <c r="B7" s="48" t="s">
+        <v>69</v>
       </c>
-      <c r="C7" s="113"/>
-      <c r="D7" s="114"/>
-      <c r="E7" s="114"/>
-      <c r="F7" s="114"/>
-      <c r="G7" s="115"/>
+      <c r="C7" s="111"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="112"/>
+      <c r="G7" s="113"/>
     </row>
     <row r="9" spans="1:13" ht="39.75" customHeight="1">
       <c r="A9" s="33" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="33" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="H9" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="33" t="s">
-        <v>14</v>
-      </c>
       <c r="I9" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J9" s="33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K9" s="33" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="L9" s="34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M9" s="34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -46358,7 +46090,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="K11" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L11" s="24"/>
       <c r="M11" s="24"/>
@@ -46379,4 +46111,179 @@
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="35"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="37">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed Template to allow Bind to @System@
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@3346 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: f57fbbbffbbc2c3d9c98cc2da7aba2d4b3397f68
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgalbraith\workspace\Semoss\export\Reports\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -403,10 +398,10 @@
 6. System Interface Requirements</t>
   </si>
   <si>
-    <t>This section displays the data objects that @SYSTEM@ creates, reads, or modifies. This information is used in concert with the @SYSTEM@ interface control documents to define what data @SYSTEM is a source of record of and what data @SYSTEM@ consumes.</t>
+    <t>C/R/M</t>
   </si>
   <si>
-    <t>C/R/M</t>
+    <t>This section displays the data objects that @SYSTEM@ creates, reads, or modifies. This information is used in concert with the @SYSTEM@ interface control documents to define what data @SYSTEM@ is a source of record of and what data @SYSTEM@ consumes.</t>
   </si>
 </sst>
 </file>
@@ -1440,11 +1435,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="419586000"/>
-        <c:axId val="419586392"/>
+        <c:axId val="205335168"/>
+        <c:axId val="205374208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="419586000"/>
+        <c:axId val="205335168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1454,7 +1449,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="419586392"/>
+        <c:crossAx val="205374208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1462,7 +1457,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="419586392"/>
+        <c:axId val="205374208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1473,7 +1468,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="419586000"/>
+        <c:crossAx val="205335168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1606,11 +1601,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="419587176"/>
-        <c:axId val="419587568"/>
+        <c:axId val="208122624"/>
+        <c:axId val="208124160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="419587176"/>
+        <c:axId val="208122624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1620,7 +1615,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="419587568"/>
+        <c:crossAx val="208124160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1628,7 +1623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="419587568"/>
+        <c:axId val="208124160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1639,7 +1634,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="419587176"/>
+        <c:crossAx val="208122624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1920,11 +1915,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="419588352"/>
-        <c:axId val="419588744"/>
+        <c:axId val="213357696"/>
+        <c:axId val="213360000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="419588352"/>
+        <c:axId val="213357696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1934,7 +1929,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="419588744"/>
+        <c:crossAx val="213360000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1942,7 +1937,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="419588744"/>
+        <c:axId val="213360000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1953,7 +1948,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="419588352"/>
+        <c:crossAx val="213357696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -44239,7 +44234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -44274,7 +44269,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -45731,8 +45726,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection sqref="A1:J7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -45763,7 +45758,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="103" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C4" s="104"/>
       <c r="D4" s="104"/>
@@ -45779,7 +45774,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -45939,8 +45934,8 @@
   </sheetPr>
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Changed 'Instructions' to 'Report Overview'
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@3349 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions" sheetId="33" r:id="rId1"/>
+    <sheet name="Report Overview" sheetId="33" r:id="rId1"/>
     <sheet name="System Overview" sheetId="21" r:id="rId2"/>
     <sheet name="Software Lifecycles" sheetId="22" r:id="rId3"/>
     <sheet name="Hardware Lifecycles" sheetId="23" r:id="rId4"/>
@@ -198,9 +198,6 @@
   </si>
   <si>
     <t>System Interfaces</t>
-  </si>
-  <si>
-    <t>This section displays data objects for which @SYSTEM@ is Source of Record (SOR) and which of those that DHMSM is also SOR for.</t>
   </si>
   <si>
     <t>System Name</t>
@@ -402,6 +399,9 @@
   </si>
   <si>
     <t>This section displays the data objects that @SYSTEM@ creates, reads, or modifies. This information is used in concert with the @SYSTEM@ interface control documents to define what data @SYSTEM@ is a source of record of and what data @SYSTEM@ consumes.</t>
+  </si>
+  <si>
+    <t>This section displays data objects for which @SYSTEM@ is Source of Record (SOR) and which of those DHMSM is expected to become the SOR for in the future.</t>
   </si>
 </sst>
 </file>
@@ -1435,11 +1435,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="205335168"/>
-        <c:axId val="205374208"/>
+        <c:axId val="233594880"/>
+        <c:axId val="233596416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="205335168"/>
+        <c:axId val="233594880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,7 +1449,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205374208"/>
+        <c:crossAx val="233596416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1457,7 +1457,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="205374208"/>
+        <c:axId val="233596416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1468,7 +1468,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205335168"/>
+        <c:crossAx val="233594880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1601,11 +1601,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="208122624"/>
-        <c:axId val="208124160"/>
+        <c:axId val="233904384"/>
+        <c:axId val="233906176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="208122624"/>
+        <c:axId val="233904384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,7 +1615,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208124160"/>
+        <c:crossAx val="233906176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1623,7 +1623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208124160"/>
+        <c:axId val="233906176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1634,7 +1634,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208122624"/>
+        <c:crossAx val="233904384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1915,11 +1915,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="213357696"/>
-        <c:axId val="213360000"/>
+        <c:axId val="234114048"/>
+        <c:axId val="234119936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="213357696"/>
+        <c:axId val="234114048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1929,7 +1929,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213360000"/>
+        <c:crossAx val="234119936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1937,7 +1937,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213360000"/>
+        <c:axId val="234119936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1948,7 +1948,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213357696"/>
+        <c:crossAx val="234114048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -44484,8 +44484,8 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -44498,12 +44498,12 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="32.25" customHeight="1">
       <c r="A2" s="53" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="54"/>
       <c r="C2" s="54"/>
@@ -44519,12 +44519,12 @@
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="281.25" customHeight="1">
       <c r="A4" s="55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
@@ -44540,12 +44540,12 @@
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="30" customFormat="1" ht="29.25" customHeight="1">
       <c r="A6" s="53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="54"/>
       <c r="C6" s="54"/>
@@ -44561,12 +44561,12 @@
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="134.25" customHeight="1">
       <c r="A8" s="58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -44682,11 +44682,11 @@
     <row r="2" spans="1:13" s="4" customFormat="1" ht="261.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="68"/>
       <c r="D2" s="69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" s="70"/>
       <c r="F2" s="70"/>
@@ -44716,7 +44716,7 @@
     <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="54"/>
       <c r="D4" s="54"/>
@@ -44759,7 +44759,7 @@
       </c>
       <c r="C7" s="68"/>
       <c r="D7" s="69" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="70"/>
       <c r="F7" s="70"/>
@@ -44806,15 +44806,15 @@
       </c>
       <c r="E10" s="73"/>
       <c r="F10" s="72" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="72"/>
       <c r="H10" s="86" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I10" s="87"/>
       <c r="J10" s="72" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K10" s="72"/>
       <c r="L10" s="72" t="s">
@@ -44839,7 +44839,7 @@
     </row>
     <row r="13" spans="1:13" ht="16.5">
       <c r="B13" s="74" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="75"/>
       <c r="D13" s="75"/>
@@ -44855,7 +44855,7 @@
     </row>
     <row r="14" spans="1:13" ht="51" customHeight="1">
       <c r="B14" s="80" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="81"/>
       <c r="D14" s="81"/>
@@ -44871,7 +44871,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="B15" s="83" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="84"/>
       <c r="D15" s="84"/>
@@ -44879,7 +44879,7 @@
       <c r="F15" s="84"/>
       <c r="G15" s="85"/>
       <c r="H15" s="83" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I15" s="84"/>
       <c r="J15" s="84"/>
@@ -45113,7 +45113,7 @@
     </row>
     <row r="33" spans="2:13" ht="16.5">
       <c r="B33" s="74" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C33" s="75"/>
       <c r="D33" s="75"/>
@@ -45129,7 +45129,7 @@
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
       <c r="B34" s="77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C34" s="78"/>
       <c r="D34" s="78"/>
@@ -45370,7 +45370,7 @@
     <row r="52" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A52" s="7"/>
       <c r="B52" s="74" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C52" s="75"/>
       <c r="D52" s="75"/>
@@ -45387,19 +45387,19 @@
     <row r="53" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A53" s="7"/>
       <c r="B53" s="61" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C53" s="62"/>
       <c r="D53" s="62"/>
       <c r="E53" s="63"/>
       <c r="F53" s="61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G53" s="62"/>
       <c r="H53" s="62"/>
       <c r="I53" s="63"/>
       <c r="J53" s="61" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K53" s="62"/>
       <c r="L53" s="62"/>
@@ -45487,7 +45487,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
@@ -45514,12 +45514,12 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="68.25" customHeight="1">
       <c r="A5" s="95" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="96"/>
       <c r="C5" s="96"/>
@@ -45530,7 +45530,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
@@ -45539,7 +45539,7 @@
       </c>
       <c r="B7" s="93"/>
       <c r="C7" s="89" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="90"/>
       <c r="E7" s="90"/>
@@ -45548,7 +45548,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="25.5">
@@ -45556,7 +45556,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>26</v>
@@ -45585,7 +45585,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -45650,7 +45650,7 @@
     </row>
     <row r="5" spans="1:7" ht="67.5" customHeight="1">
       <c r="A5" s="95" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="96"/>
       <c r="C5" s="96"/>
@@ -45665,7 +45665,7 @@
       </c>
       <c r="B7" s="94"/>
       <c r="C7" s="101" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="101"/>
       <c r="E7" s="101"/>
@@ -45677,7 +45677,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>26</v>
@@ -45726,8 +45726,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -45758,7 +45758,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="103" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="104"/>
       <c r="D4" s="104"/>
@@ -45774,7 +45774,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -45813,7 +45813,7 @@
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
       <c r="A2" s="102" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="102"/>
       <c r="C2" s="102"/>
@@ -45830,7 +45830,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="103" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="104"/>
       <c r="D4" s="105"/>
@@ -45843,10 +45843,10 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -45872,7 +45872,7 @@
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -45884,7 +45884,7 @@
   <sheetData>
     <row r="2" spans="1:2" ht="18">
       <c r="A2" s="102" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="102"/>
     </row>
@@ -45897,7 +45897,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -45981,7 +45981,7 @@
       <c r="B4" s="115"/>
       <c r="C4" s="116"/>
       <c r="D4" s="106" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="107"/>
       <c r="F4" s="107"/>
@@ -45995,22 +45995,22 @@
     </row>
     <row r="6" spans="1:13" ht="96.75" customHeight="1">
       <c r="A6" s="109" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="110"/>
       <c r="D6" s="110"/>
       <c r="E6" s="110"/>
       <c r="F6" s="48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6" s="110"/>
       <c r="H6" s="110"/>
       <c r="I6" s="110"/>
       <c r="J6" s="48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K6" s="110"/>
       <c r="L6" s="110"/>
@@ -46019,7 +46019,7 @@
     <row r="7" spans="1:13" ht="45" customHeight="1">
       <c r="A7" s="109"/>
       <c r="B7" s="48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="111"/>
       <c r="D7" s="112"/>
@@ -46059,13 +46059,13 @@
         <v>8</v>
       </c>
       <c r="K9" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L9" s="34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M9" s="34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -46127,21 +46127,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="35"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="37">
         <v>0</v>
@@ -46149,7 +46149,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="37">
         <v>0</v>
@@ -46157,7 +46157,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="37">
         <v>0</v>
@@ -46165,7 +46165,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="37">
         <v>0</v>
@@ -46173,20 +46173,20 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="37">
         <v>0</v>
@@ -46194,7 +46194,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="37">
         <v>0</v>
@@ -46202,7 +46202,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="37">
         <v>0</v>
@@ -46210,7 +46210,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="37">
         <v>0</v>
@@ -46218,7 +46218,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -46226,12 +46226,12 @@
         <v>2</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="37">
         <v>0</v>
@@ -46239,7 +46239,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="37">
         <v>0</v>
@@ -46247,7 +46247,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="37">
         <v>0</v>
@@ -46255,7 +46255,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" s="37">
         <v>0</v>
@@ -46263,7 +46263,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="37">
         <v>0</v>
@@ -46271,7 +46271,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25" s="37">
         <v>0</v>

</xml_diff>

<commit_message>
Updated to reflect latest input from program reviews.
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@3462 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_HPI_Transition_Report_Template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgalbraith\workspace\Semoss\export\Reports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834"/>
   </bookViews>
@@ -14,12 +19,12 @@
     <sheet name="System Data" sheetId="30" r:id="rId5"/>
     <sheet name="System BLU" sheetId="35" r:id="rId6"/>
     <sheet name="SOR Overlap With DHMSM" sheetId="28" r:id="rId7"/>
-    <sheet name="System Interfaces" sheetId="27" r:id="rId8"/>
-    <sheet name="Summary Charts" sheetId="34" r:id="rId9"/>
+    <sheet name="Future Interface Development" sheetId="36" r:id="rId8"/>
+    <sheet name="Future Interface Decommission" sheetId="37" r:id="rId9"/>
+    <sheet name="Future Interface Sustainment" sheetId="38" r:id="rId10"/>
+    <sheet name="Summary Charts" sheetId="34" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
-    <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
     <externalReference r:id="rId14"/>
@@ -29,6 +34,9 @@
     <externalReference r:id="rId18"/>
     <externalReference r:id="rId19"/>
     <externalReference r:id="rId20"/>
+    <externalReference r:id="rId21"/>
+    <externalReference r:id="rId22"/>
+    <externalReference r:id="rId23"/>
   </externalReferences>
   <definedNames>
     <definedName name="Additional">[1]Data!$D$3:$D$15</definedName>
@@ -55,6 +63,9 @@
     <definedName name="FY15_Total">'[2]Fiscal Year Breakdown'!$AO$18</definedName>
     <definedName name="HW" localSheetId="0">[4]SiteDB2!$L$2:$L$330</definedName>
     <definedName name="HW">[5]SiteDB2!$L$2:$L$330</definedName>
+    <definedName name="I_O" localSheetId="8">#REF!</definedName>
+    <definedName name="I_O" localSheetId="7">#REF!</definedName>
+    <definedName name="I_O" localSheetId="9">#REF!</definedName>
     <definedName name="I_O" localSheetId="0">#REF!</definedName>
     <definedName name="I_O" localSheetId="5">#REF!</definedName>
     <definedName name="I_O" localSheetId="4">#REF!</definedName>
@@ -74,7 +85,6 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Software Lifecycles'!$9:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">'SOR Overlap With DHMSM'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'System Data'!$6:$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="7">'System Interfaces'!$9:$9</definedName>
     <definedName name="Priority3">[6]Data1!$B$4:$B$6</definedName>
     <definedName name="ProcContractMonths">'[2]New Timeline'!$A$22</definedName>
     <definedName name="RangeBLU">[7]BLUBackEnd!$G$5:$G$49</definedName>
@@ -91,6 +101,9 @@
     <definedName name="SW">[5]SiteDB2!$K$2:$K$392</definedName>
     <definedName name="System">'[10]2. System Information'!$D$3</definedName>
     <definedName name="Teams">[2]Cheat!$A$38:$A$39</definedName>
+    <definedName name="Type" localSheetId="8">#REF!</definedName>
+    <definedName name="Type" localSheetId="7">#REF!</definedName>
+    <definedName name="Type" localSheetId="9">#REF!</definedName>
     <definedName name="Type" localSheetId="0">#REF!</definedName>
     <definedName name="Type" localSheetId="5">#REF!</definedName>
     <definedName name="Type" localSheetId="4">#REF!</definedName>
@@ -105,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="83">
   <si>
     <t>Garrison / Theater</t>
   </si>
@@ -129,15 +142,6 @@
   </si>
   <si>
     <t>DHMSM SOR?</t>
-  </si>
-  <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>Interfacing System</t>
-  </si>
-  <si>
-    <t>Interface</t>
   </si>
   <si>
     <t>Format</t>
@@ -179,16 +183,10 @@
     <t>Annual Hardware Sustainment Cost</t>
   </si>
   <si>
-    <t>Probability of Interfacing System</t>
-  </si>
-  <si>
     <t xml:space="preserve">System </t>
   </si>
   <si>
     <t>Lifecycle Phase</t>
-  </si>
-  <si>
-    <t>DHMSM Provide / Consume</t>
   </si>
   <si>
     <t>System Description</t>
@@ -197,22 +195,10 @@
     <t>System Data</t>
   </si>
   <si>
-    <t>System Interfaces</t>
-  </si>
-  <si>
     <t>System Name</t>
   </si>
   <si>
     <t>Report Overview</t>
-  </si>
-  <si>
-    <t>This section displays the current @SYSTEM@ interfaces and how they are affected by DHMSM deployment.</t>
-  </si>
-  <si>
-    <t>Direct Cost</t>
-  </si>
-  <si>
-    <t>Indirect Cost</t>
   </si>
   <si>
     <t>Average Daily Transaction Count</t>
@@ -327,21 +313,6 @@
     <t>Recommendation</t>
   </si>
   <si>
-    <t>Legend</t>
-  </si>
-  <si>
-    <t>Direct Integration</t>
-  </si>
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>Indirect Integration</t>
-  </si>
-  <si>
-    <t>Removed Legacy Interfaces</t>
-  </si>
-  <si>
     <t>The Office of Transition Management (OTM) Transition Application Planning (TAP) coordinated with the Defense Health Clinical Systems (DHCS) and Defense Health Services Systems (DHSS) program offices, in addition to the tri-Services, to collect technical and functional data regarding their information systems, in order to fully characterize the legacy DHA IM/IT portfolio. 
 Using this data, OTM provided detailed analysis regarding each legacy system to the Functional Advisory Council (FAC), which made transition decisions that define if each system would be replaced by the future-state EHR (high probability systems) or would endure to support the future-state EHR (low probability systems).
 This report focuses on high probability systems that will require integration with the future-state EHR until FOC when they will be completely replaced by the future-state EHR. It provides analytical insights that specify the activities required for the system highlighted in this report to transition to the future state environment.</t>
@@ -403,14 +374,40 @@
   <si>
     <t>This section displays data objects for which @SYSTEM@ is Source of Record (SOR) and which of those DHMSM is expected to become the SOR for in the future.</t>
   </si>
+  <si>
+    <t>Future Interface Development</t>
+  </si>
+  <si>
+    <t>This section defines the future interfaces that must be developed for @SYSTEM@ in order to support continuity of operations into the future-state environment.</t>
+  </si>
+  <si>
+    <t>Upstream System</t>
+  </si>
+  <si>
+    <t>Downstream System</t>
+  </si>
+  <si>
+    <t>ICD Name</t>
+  </si>
+  <si>
+    <t>Future Interface Decommissioning</t>
+  </si>
+  <si>
+    <t>This section defines the current interfaces for @SYSTEM@ that will be retired in support of the future-state architecture as the system is transitioned to the future-state environment.</t>
+  </si>
+  <si>
+    <t>Future Interface Sustainment</t>
+  </si>
+  <si>
+    <t>This section defines the current interfaces for @SYSTEM@ that will continue to be supported as the system is transitioned to the future-state environment.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -583,16 +580,17 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Impact"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
-      <sz val="10"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Impact"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -640,7 +638,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -799,7 +797,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -860,8 +858,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -909,16 +908,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="48" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="21" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -938,9 +929,6 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -954,9 +942,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -993,45 +978,6 @@
     <xf numFmtId="0" fontId="24" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1059,6 +1005,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1068,11 +1023,41 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1128,41 +1113,26 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="1" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="52">
     <cellStyle name="%" xfId="2"/>
     <cellStyle name="% 2" xfId="3"/>
     <cellStyle name="Currency" xfId="49" builtinId="4"/>
@@ -1204,6 +1174,7 @@
     <cellStyle name="Normal 6_System-BLIO" xfId="37"/>
     <cellStyle name="Normal 7" xfId="48"/>
     <cellStyle name="Normal 8" xfId="50"/>
+    <cellStyle name="Normal 9" xfId="51"/>
     <cellStyle name="Percent 2" xfId="38"/>
     <cellStyle name="Percent 2 2" xfId="39"/>
     <cellStyle name="Percent 2 2 2" xfId="40"/>
@@ -1435,11 +1406,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="233594880"/>
-        <c:axId val="233596416"/>
+        <c:axId val="477848592"/>
+        <c:axId val="477848984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="233594880"/>
+        <c:axId val="477848592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,7 +1420,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233596416"/>
+        <c:crossAx val="477848984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1457,7 +1428,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="233596416"/>
+        <c:axId val="477848984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1468,7 +1439,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233594880"/>
+        <c:crossAx val="477848592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1601,11 +1572,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="233904384"/>
-        <c:axId val="233906176"/>
+        <c:axId val="399735816"/>
+        <c:axId val="399735424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="233904384"/>
+        <c:axId val="399735816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,7 +1586,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233906176"/>
+        <c:crossAx val="399735424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1623,7 +1594,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="233906176"/>
+        <c:axId val="399735424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1634,7 +1605,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233904384"/>
+        <c:crossAx val="399735816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1915,11 +1886,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="234114048"/>
-        <c:axId val="234119936"/>
+        <c:axId val="399732288"/>
+        <c:axId val="477849768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="234114048"/>
+        <c:axId val="399732288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1929,7 +1900,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="234119936"/>
+        <c:crossAx val="477849768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1937,7 +1908,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="234119936"/>
+        <c:axId val="477849768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1948,7 +1919,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="234114048"/>
+        <c:crossAx val="399732288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2064,201 +2035,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1447800</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>229072</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1371798</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1022840</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4000500" y="1267297"/>
-          <a:ext cx="2286198" cy="793768"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>200026</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>110190</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>940605</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1141723</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7591426" y="1148415"/>
-          <a:ext cx="2531279" cy="1031533"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>462145</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1194762</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Picture 21"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12001500" y="1095375"/>
-          <a:ext cx="2538595" cy="1137612"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1467048</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1022368</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1733550" y="1266825"/>
-          <a:ext cx="2286198" cy="793768"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>541237</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1819275" y="2305050"/>
-          <a:ext cx="6705600" cy="503137"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -3262,6 +3038,39 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Report Overview"/>
+      <sheetName val="System Overview"/>
+      <sheetName val="Software Lifecycles"/>
+      <sheetName val="Hardware Lifecycles"/>
+      <sheetName val="System Data"/>
+      <sheetName val="System BLU"/>
+      <sheetName val="SOR Overlap With DHMSM"/>
+      <sheetName val="Future Interface Development"/>
+      <sheetName val="Future Interface Decommission"/>
+      <sheetName val="Future Interface Sustainment"/>
+      <sheetName val="Summary Charts"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -44234,7 +44043,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -44269,7 +44078,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -44485,156 +44294,156 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="29" customWidth="1"/>
-    <col min="2" max="11" width="9.140625" style="29"/>
-    <col min="12" max="12" width="33.28515625" style="29" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="29"/>
+    <col min="1" max="1" width="17.5703125" style="25" customWidth="1"/>
+    <col min="2" max="11" width="9.140625" style="25"/>
+    <col min="12" max="12" width="33.28515625" style="25" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="32.25" customHeight="1">
-      <c r="A2" s="53" t="s">
-        <v>43</v>
+      <c r="A2" s="47" t="s">
+        <v>34</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="281.25" customHeight="1">
-      <c r="A4" s="55" t="s">
-        <v>72</v>
+      <c r="A4" s="49" t="s">
+        <v>58</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="57"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="51"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="30" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A6" s="53" t="s">
-        <v>45</v>
+    <row r="6" spans="1:12" s="26" customFormat="1" ht="29.25" customHeight="1">
+      <c r="A6" s="47" t="s">
+        <v>36</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="134.25" customHeight="1">
-      <c r="A8" s="58" t="s">
-        <v>84</v>
+      <c r="A8" s="52" t="s">
+        <v>70</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="60"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="54"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -44649,6 +44458,292 @@
     <oddHeader>&amp;C&amp;F
 &amp;A</oddHeader>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF366092"/>
+  </sheetPr>
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="7" width="13.140625" style="105" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="18">
+      <c r="A2" s="100" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="36.75" customHeight="1">
+      <c r="A4" s="101" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="101"/>
+      <c r="C4" s="102" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="30">
+      <c r="A6" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="103" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="103" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="103" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="103" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="103" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="104"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="104"/>
+      <c r="G7" s="104"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="30"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="32">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
@@ -44681,22 +44776,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="261.75" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="67" t="s">
-        <v>32</v>
+      <c r="B2" s="75" t="s">
+        <v>26</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="69" t="s">
-        <v>71</v>
+      <c r="C2" s="76"/>
+      <c r="D2" s="64" t="s">
+        <v>57</v>
       </c>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="71"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="66"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -44715,20 +44810,20 @@
     </row>
     <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="53" t="s">
-        <v>31</v>
+      <c r="B4" s="47" t="s">
+        <v>25</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
     </row>
     <row r="5" spans="1:13" ht="7.5" customHeight="1">
       <c r="A5" s="5"/>
@@ -44754,22 +44849,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="67" t="s">
-        <v>28</v>
+      <c r="B7" s="75" t="s">
+        <v>23</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="69" t="s">
-        <v>46</v>
+      <c r="C7" s="76"/>
+      <c r="D7" s="64" t="s">
+        <v>37</v>
       </c>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="70"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="71"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="66"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -44780,660 +44875,654 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="76"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="57"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72" t="s">
+      <c r="C10" s="70"/>
+      <c r="D10" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="72" t="s">
-        <v>36</v>
+      <c r="E10" s="77"/>
+      <c r="F10" s="70" t="s">
+        <v>27</v>
       </c>
-      <c r="G10" s="72"/>
-      <c r="H10" s="86" t="s">
-        <v>37</v>
+      <c r="G10" s="70"/>
+      <c r="H10" s="71" t="s">
+        <v>28</v>
       </c>
-      <c r="I10" s="87"/>
-      <c r="J10" s="72" t="s">
-        <v>38</v>
+      <c r="I10" s="72"/>
+      <c r="J10" s="70" t="s">
+        <v>29</v>
       </c>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72" t="s">
+      <c r="K10" s="70"/>
+      <c r="L10" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="72"/>
+      <c r="M10" s="70"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="66"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="74"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="74"/>
     </row>
     <row r="13" spans="1:13" ht="16.5">
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="57"/>
+    </row>
+    <row r="14" spans="1:13" ht="51" customHeight="1">
+      <c r="B14" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="63"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="B15" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="75"/>
-      <c r="L13" s="75"/>
-      <c r="M13" s="76"/>
-    </row>
-    <row r="14" spans="1:13" ht="51" customHeight="1">
-      <c r="B14" s="80" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="81"/>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="82"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="B15" s="83" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="83" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="84"/>
-      <c r="L15" s="84"/>
-      <c r="M15" s="85"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="69"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="41"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="36"/>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="44"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="39"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="42"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="44"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="39"/>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="42"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="44"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="39"/>
     </row>
     <row r="20" spans="2:13">
-      <c r="B20" s="42"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="44"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="39"/>
     </row>
     <row r="21" spans="2:13">
-      <c r="B21" s="42"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="44"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="39"/>
     </row>
     <row r="22" spans="2:13">
-      <c r="B22" s="42"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="44"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="39"/>
     </row>
     <row r="23" spans="2:13">
-      <c r="B23" s="42"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="44"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="39"/>
     </row>
     <row r="24" spans="2:13">
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="44"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="39"/>
     </row>
     <row r="25" spans="2:13">
-      <c r="B25" s="42"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="44"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="39"/>
     </row>
     <row r="26" spans="2:13">
-      <c r="B26" s="42"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="44"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="39"/>
     </row>
     <row r="27" spans="2:13">
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="44"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="39"/>
     </row>
     <row r="28" spans="2:13">
-      <c r="B28" s="42"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="44"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="39"/>
     </row>
     <row r="29" spans="2:13">
-      <c r="B29" s="42"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="44"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="39"/>
     </row>
     <row r="30" spans="2:13">
-      <c r="B30" s="42"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="44"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="39"/>
     </row>
     <row r="31" spans="2:13">
-      <c r="B31" s="45"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="47"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="42"/>
     </row>
     <row r="33" spans="2:13" ht="16.5">
-      <c r="B33" s="74" t="s">
-        <v>57</v>
+      <c r="B33" s="55" t="s">
+        <v>48</v>
       </c>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="75"/>
-      <c r="I33" s="75"/>
-      <c r="J33" s="75"/>
-      <c r="K33" s="75"/>
-      <c r="L33" s="75"/>
-      <c r="M33" s="76"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="57"/>
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B34" s="77" t="s">
-        <v>63</v>
+      <c r="B34" s="58" t="s">
+        <v>54</v>
       </c>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
-      <c r="J34" s="78"/>
-      <c r="K34" s="78"/>
-      <c r="L34" s="78"/>
-      <c r="M34" s="79"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="59"/>
+      <c r="J34" s="59"/>
+      <c r="K34" s="59"/>
+      <c r="L34" s="59"/>
+      <c r="M34" s="60"/>
     </row>
     <row r="35" spans="2:13">
-      <c r="B35" s="39"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="40"/>
-      <c r="K35" s="40"/>
-      <c r="L35" s="40"/>
-      <c r="M35" s="41"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="36"/>
     </row>
     <row r="36" spans="2:13">
-      <c r="B36" s="42"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="43"/>
-      <c r="M36" s="44"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="38"/>
+      <c r="L36" s="38"/>
+      <c r="M36" s="39"/>
     </row>
     <row r="37" spans="2:13">
-      <c r="B37" s="42"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="43"/>
-      <c r="M37" s="44"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="38"/>
+      <c r="M37" s="39"/>
     </row>
     <row r="38" spans="2:13">
-      <c r="B38" s="42"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="43"/>
-      <c r="K38" s="43"/>
-      <c r="L38" s="43"/>
-      <c r="M38" s="44"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="38"/>
+      <c r="K38" s="38"/>
+      <c r="L38" s="38"/>
+      <c r="M38" s="39"/>
     </row>
     <row r="39" spans="2:13">
-      <c r="B39" s="42"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="43"/>
-      <c r="L39" s="43"/>
-      <c r="M39" s="44"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
+      <c r="K39" s="38"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="39"/>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="42"/>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
-      <c r="J40" s="43"/>
-      <c r="K40" s="43"/>
-      <c r="L40" s="43"/>
-      <c r="M40" s="44"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38"/>
+      <c r="K40" s="38"/>
+      <c r="L40" s="38"/>
+      <c r="M40" s="39"/>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="42"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="43"/>
-      <c r="L41" s="43"/>
-      <c r="M41" s="44"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="38"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="39"/>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="42"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
-      <c r="K42" s="43"/>
-      <c r="L42" s="43"/>
-      <c r="M42" s="44"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="38"/>
+      <c r="K42" s="38"/>
+      <c r="L42" s="38"/>
+      <c r="M42" s="39"/>
     </row>
     <row r="43" spans="2:13">
-      <c r="B43" s="42"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="43"/>
-      <c r="L43" s="43"/>
-      <c r="M43" s="44"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
+      <c r="K43" s="38"/>
+      <c r="L43" s="38"/>
+      <c r="M43" s="39"/>
     </row>
     <row r="44" spans="2:13">
-      <c r="B44" s="42"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="43"/>
-      <c r="L44" s="43"/>
-      <c r="M44" s="44"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="38"/>
+      <c r="K44" s="38"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="39"/>
     </row>
     <row r="45" spans="2:13">
-      <c r="B45" s="42"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="43"/>
-      <c r="L45" s="43"/>
-      <c r="M45" s="44"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="38"/>
+      <c r="K45" s="38"/>
+      <c r="L45" s="38"/>
+      <c r="M45" s="39"/>
     </row>
     <row r="46" spans="2:13">
-      <c r="B46" s="42"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
-      <c r="K46" s="43"/>
-      <c r="L46" s="43"/>
-      <c r="M46" s="44"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
+      <c r="K46" s="38"/>
+      <c r="L46" s="38"/>
+      <c r="M46" s="39"/>
     </row>
     <row r="47" spans="2:13">
-      <c r="B47" s="42"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="43"/>
-      <c r="J47" s="43"/>
-      <c r="K47" s="43"/>
-      <c r="L47" s="43"/>
-      <c r="M47" s="44"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="38"/>
+      <c r="K47" s="38"/>
+      <c r="L47" s="38"/>
+      <c r="M47" s="39"/>
     </row>
     <row r="48" spans="2:13">
-      <c r="B48" s="42"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
-      <c r="J48" s="43"/>
-      <c r="K48" s="43"/>
-      <c r="L48" s="43"/>
-      <c r="M48" s="44"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="38"/>
+      <c r="K48" s="38"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="39"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="B49" s="42"/>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="43"/>
-      <c r="M49" s="44"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="38"/>
+      <c r="K49" s="38"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="39"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="B50" s="45"/>
-      <c r="C50" s="46"/>
-      <c r="D50" s="46"/>
-      <c r="E50" s="46"/>
-      <c r="F50" s="46"/>
-      <c r="G50" s="46"/>
-      <c r="H50" s="46"/>
-      <c r="I50" s="46"/>
-      <c r="J50" s="46"/>
-      <c r="K50" s="46"/>
-      <c r="L50" s="46"/>
-      <c r="M50" s="47"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="41"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="41"/>
+      <c r="J50" s="41"/>
+      <c r="K50" s="41"/>
+      <c r="L50" s="41"/>
+      <c r="M50" s="42"/>
     </row>
     <row r="52" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A52" s="7"/>
-      <c r="B52" s="74" t="s">
-        <v>73</v>
+      <c r="B52" s="55" t="s">
+        <v>59</v>
       </c>
-      <c r="C52" s="75"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="75"/>
-      <c r="G52" s="75"/>
-      <c r="H52" s="75"/>
-      <c r="I52" s="75"/>
-      <c r="J52" s="75"/>
-      <c r="K52" s="75"/>
-      <c r="L52" s="75"/>
-      <c r="M52" s="76"/>
+      <c r="C52" s="56"/>
+      <c r="D52" s="56"/>
+      <c r="E52" s="56"/>
+      <c r="F52" s="56"/>
+      <c r="G52" s="56"/>
+      <c r="H52" s="56"/>
+      <c r="I52" s="56"/>
+      <c r="J52" s="56"/>
+      <c r="K52" s="56"/>
+      <c r="L52" s="56"/>
+      <c r="M52" s="57"/>
     </row>
     <row r="53" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A53" s="7"/>
-      <c r="B53" s="61" t="s">
-        <v>75</v>
+      <c r="B53" s="78" t="s">
+        <v>61</v>
       </c>
-      <c r="C53" s="62"/>
-      <c r="D53" s="62"/>
-      <c r="E53" s="63"/>
-      <c r="F53" s="61" t="s">
-        <v>76</v>
+      <c r="C53" s="79"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="80"/>
+      <c r="F53" s="78" t="s">
+        <v>62</v>
       </c>
-      <c r="G53" s="62"/>
-      <c r="H53" s="62"/>
-      <c r="I53" s="63"/>
-      <c r="J53" s="61" t="s">
-        <v>74</v>
+      <c r="G53" s="79"/>
+      <c r="H53" s="79"/>
+      <c r="I53" s="80"/>
+      <c r="J53" s="78" t="s">
+        <v>60</v>
       </c>
-      <c r="K53" s="62"/>
-      <c r="L53" s="62"/>
-      <c r="M53" s="63"/>
+      <c r="K53" s="79"/>
+      <c r="L53" s="79"/>
+      <c r="M53" s="80"/>
     </row>
     <row r="54" spans="1:13" ht="42.75" customHeight="1">
       <c r="A54" s="5"/>
-      <c r="B54" s="64"/>
-      <c r="C54" s="65"/>
-      <c r="D54" s="65"/>
-      <c r="E54" s="66"/>
-      <c r="F54" s="64"/>
-      <c r="G54" s="65"/>
-      <c r="H54" s="65"/>
-      <c r="I54" s="66"/>
-      <c r="J54" s="64"/>
-      <c r="K54" s="65"/>
-      <c r="L54" s="65"/>
-      <c r="M54" s="66"/>
+      <c r="B54" s="73"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81"/>
+      <c r="E54" s="74"/>
+      <c r="F54" s="73"/>
+      <c r="G54" s="81"/>
+      <c r="H54" s="81"/>
+      <c r="I54" s="74"/>
+      <c r="J54" s="73"/>
+      <c r="K54" s="81"/>
+      <c r="L54" s="81"/>
+      <c r="M54" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B52:M52"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="F54:I54"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -45447,12 +45536,18 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="B52:M52"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45487,105 +45582,105 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="88" t="s">
-        <v>14</v>
+      <c r="A2" s="82" t="s">
+        <v>11</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
-      <c r="A3" s="94" t="s">
-        <v>25</v>
+      <c r="A3" s="88" t="s">
+        <v>21</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="68.25" customHeight="1">
-      <c r="A5" s="95" t="s">
-        <v>78</v>
+      <c r="A5" s="89" t="s">
+        <v>64</v>
       </c>
-      <c r="B5" s="96"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="97"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="91"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A7" s="92" t="s">
-        <v>19</v>
+      <c r="A7" s="86" t="s">
+        <v>16</v>
       </c>
-      <c r="B7" s="93"/>
-      <c r="C7" s="89" t="s">
-        <v>41</v>
+      <c r="B7" s="87"/>
+      <c r="C7" s="83" t="s">
+        <v>32</v>
       </c>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="91"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="85"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="25.5">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="33" t="s">
+      <c r="G9" s="29" t="s">
         <v>18</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="23"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="26"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="26"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -45627,82 +45722,82 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="98" t="s">
-        <v>20</v>
+      <c r="A2" s="92" t="s">
+        <v>17</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="100"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="94"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
     </row>
     <row r="5" spans="1:7" ht="67.5" customHeight="1">
-      <c r="A5" s="95" t="s">
-        <v>79</v>
+      <c r="A5" s="89" t="s">
+        <v>65</v>
       </c>
-      <c r="B5" s="96"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="97"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="91"/>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="88" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="88"/>
+      <c r="C7" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="95"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+    </row>
+    <row r="9" spans="1:7" ht="25.5">
+      <c r="A9" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="101" t="s">
-        <v>42</v>
+      <c r="B9" s="29" t="s">
+        <v>30</v>
       </c>
-      <c r="D7" s="101"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
-    </row>
-    <row r="9" spans="1:7" ht="25.5">
-      <c r="A9" s="33" t="s">
+      <c r="C9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>39</v>
+      <c r="D9" s="29" t="s">
+        <v>13</v>
       </c>
-      <c r="C9" s="33" t="s">
-        <v>26</v>
+      <c r="E9" s="29" t="s">
+        <v>14</v>
       </c>
-      <c r="D9" s="33" t="s">
-        <v>16</v>
+      <c r="F9" s="29" t="s">
+        <v>15</v>
       </c>
-      <c r="E9" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>23</v>
+      <c r="G9" s="29" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="23"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="26"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="26"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -45740,46 +45835,46 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1"/>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="102" t="s">
-        <v>29</v>
+      <c r="A2" s="96" t="s">
+        <v>24</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
     </row>
     <row r="4" spans="1:10" ht="53.25" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="103" t="s">
-        <v>86</v>
+      <c r="B4" s="97" t="s">
+        <v>72</v>
       </c>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="105"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="99"/>
     </row>
     <row r="6" spans="1:10" ht="39.75" customHeight="1">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="33" t="s">
-        <v>85</v>
+      <c r="B6" s="29" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -45812,46 +45907,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="102" t="s">
-        <v>80</v>
+      <c r="A2" s="96" t="s">
+        <v>66</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
     </row>
     <row r="4" spans="1:10" ht="45.75" customHeight="1">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="103" t="s">
-        <v>81</v>
+      <c r="B4" s="97" t="s">
+        <v>67</v>
       </c>
-      <c r="C4" s="104"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="33" t="s">
-        <v>82</v>
+      <c r="A6" s="29" t="s">
+        <v>68</v>
       </c>
-      <c r="B6" s="33" t="s">
-        <v>83</v>
+      <c r="B6" s="29" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -45883,10 +45978,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18">
-      <c r="A2" s="102" t="s">
-        <v>44</v>
+      <c r="A2" s="96" t="s">
+        <v>35</v>
       </c>
-      <c r="B2" s="102"/>
+      <c r="B2" s="96"/>
     </row>
     <row r="3" spans="1:2" ht="18">
       <c r="A3" s="12"/>
@@ -45897,7 +45992,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -45905,10 +46000,10 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="29" t="s">
         <v>7</v>
       </c>
     </row>
@@ -45930,354 +46025,240 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF366092"/>
-    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15" style="21" customWidth="1"/>
-    <col min="13" max="13" width="16" style="21" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="7" width="13.140625" style="105" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" style="105" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" customHeight="1"/>
-    <row r="2" spans="1:13" ht="18" customHeight="1">
-      <c r="A2" s="102" t="s">
-        <v>30</v>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="18">
+      <c r="A2" s="100" t="s">
+        <v>74</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
     </row>
-    <row r="4" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A4" s="114" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="32.25" customHeight="1">
+      <c r="A4" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="115"/>
-      <c r="C4" s="116"/>
-      <c r="D4" s="106" t="s">
-        <v>33</v>
+      <c r="B4" s="101"/>
+      <c r="C4" s="102" t="s">
+        <v>75</v>
       </c>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
-      <c r="J4" s="107"/>
-      <c r="K4" s="107"/>
-      <c r="L4" s="107"/>
-      <c r="M4" s="108"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
     </row>
-    <row r="6" spans="1:13" ht="96.75" customHeight="1">
-      <c r="A6" s="109" t="s">
-        <v>66</v>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="103" t="s">
+        <v>76</v>
       </c>
-      <c r="B6" s="48" t="s">
-        <v>67</v>
+      <c r="B6" s="103" t="s">
+        <v>77</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="48" t="s">
-        <v>69</v>
+      <c r="C6" s="103" t="s">
+        <v>78</v>
       </c>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="48" t="s">
-        <v>70</v>
+      <c r="D6" s="103" t="s">
+        <v>6</v>
       </c>
-      <c r="K6" s="110"/>
-      <c r="L6" s="110"/>
-      <c r="M6" s="110"/>
-    </row>
-    <row r="7" spans="1:13" ht="45" customHeight="1">
-      <c r="A7" s="109"/>
-      <c r="B7" s="48" t="s">
-        <v>68</v>
+      <c r="E6" s="103" t="s">
+        <v>8</v>
       </c>
-      <c r="C7" s="111"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="113"/>
-    </row>
-    <row r="9" spans="1:13" ht="39.75" customHeight="1">
-      <c r="A9" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="33" t="s">
+      <c r="F6" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="33" t="s">
+      <c r="G6" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="L9" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" s="34" t="s">
-        <v>35</v>
+      <c r="H6" s="103" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="K11" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
+    <row r="7" spans="1:8">
+      <c r="A7" s="104"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="104"/>
+      <c r="G7" s="104"/>
+      <c r="H7" s="104"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="D4:M4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A4:C4"/>
+  <mergeCells count="3">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:H4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="53" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFFF0000"/>
+    <tabColor rgb="FF366092"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="38.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="7" width="13.140625" style="105" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" style="105" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="38" t="s">
-        <v>48</v>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="18">
+      <c r="A2" s="100" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="36" customHeight="1">
+      <c r="A4" s="101" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="101"/>
+      <c r="C4" s="102" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="103" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="103" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="103" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="103" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="103" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="103" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="35"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="38" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="37">
-        <v>0</v>
-      </c>
+    <row r="7" spans="1:8">
+      <c r="A7" s="104"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="104"/>
+      <c r="G7" s="104"/>
+      <c r="H7" s="104"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:H4"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>